<commit_message>
update faktenblatt, fixes for KW/isoweek
</commit_message>
<xml_diff>
--- a/data/klinische_aspekte.xlsx
+++ b/data/klinische_aspekte.xlsx
@@ -1,9 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20367"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713DB5FF-39F4-44A0-9D24-2F5B6B4041F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20368"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Wissdaten\RKI_nCoV-Lage\3.Kommunikation\3.7.Lageberichte\2021-01-05\Dienstagstabellen für Webmaster\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF18C822-CAF0-420F-B7F2-BCDD0010CCFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" activeTab="1" xr2:uid="{E7020DAF-D42D-4B3D-9581-E23C135CB659}"/>
   </bookViews>
@@ -21,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>KW</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Fälle gesamt</t>
   </si>
@@ -59,10 +61,16 @@
     <t>Anteil Verstorben</t>
   </si>
   <si>
-    <t>Die Tabelle zeigt die dem RKI übermittelten COVID-19-Fälle nach Meldewoche und nach Geschlecht sowie Anteile mit für COVID-19 relevanten Symptomen, Anteile Hospitalisierter und Verstorbener für die Meldewochen KW 10 – 51. Eine grafische Darstellung der Daten befindt sich im Lagebericht unter dem Abschnitt "klinische Aspekte".</t>
+    <t>Die dem RKI übermittelten COVID-19-Fälle nach Meldewoche und nach Geschlecht sowie Anteile mit für COVID-19 relevanten Symptomen, Anteile Hospitalisierter und Verstorbener für die Meldewochen KW 10 – 52</t>
   </si>
   <si>
-    <t>Die dem RKI übermittelten COVID-19-Fälle nach Meldewoche und nach Geschlecht sowie Anteile mit für COVID-19 relevanten Symptomen, Anteile Hospitalisierter und Verstorbener für die Meldewochen KW 10 – 52</t>
+    <t>Meldejahr</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>Die Tabelle zeigt die dem RKI übermittelten COVID-19-Fälle nach Meldewoche und nach Geschlecht sowie Anteile mit für COVID-19 relevanten Symptomen, Anteile Hospitalisierter und Verstorbener für die Meldewochen KW 10 – 53. Eine grafische Darstellung der Daten befindt sich im Lagebericht unter dem Abschnitt "klinische Aspekte".</t>
   </si>
 </sst>
 </file>
@@ -554,7 +562,7 @@
     </row>
     <row r="5" spans="2:2" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
@@ -568,72 +576,78 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EDE9B5-504F-438C-AC14-C6D857721167}">
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48:XFD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="M3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="5">
+        <v>2020</v>
+      </c>
       <c r="C4" s="5">
         <v>10</v>
       </c>
       <c r="D4" s="6">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="E4" s="6">
         <v>42</v>
       </c>
       <c r="F4" s="7">
-        <v>0.53579418344519014</v>
+        <v>0.53527435610302354</v>
       </c>
       <c r="G4" s="7">
-        <v>0.46420581655480986</v>
+        <v>0.46472564389697646</v>
       </c>
       <c r="H4" s="8">
         <v>832</v>
@@ -654,48 +668,54 @@
         <v>12</v>
       </c>
       <c r="N4" s="10">
-        <v>1.3422818790000001E-2</v>
+        <v>1.343784994E-2</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="11">
+        <v>2020</v>
+      </c>
       <c r="C5" s="11">
         <v>11</v>
       </c>
       <c r="D5" s="12">
-        <v>6433</v>
+        <v>6434</v>
       </c>
       <c r="E5" s="13">
         <v>45</v>
       </c>
       <c r="F5" s="14">
-        <v>0.56320945420618873</v>
+        <v>0.56312189054726369</v>
       </c>
       <c r="G5" s="14">
-        <v>0.43679054579381121</v>
+        <v>0.43687810945273631</v>
       </c>
       <c r="H5" s="12">
-        <v>5779</v>
+        <v>5780</v>
       </c>
       <c r="I5" s="15">
-        <v>5.3123377747015053E-2</v>
+        <v>5.3114186851211075E-2</v>
       </c>
       <c r="J5" s="12">
-        <v>5611</v>
+        <v>5614</v>
       </c>
       <c r="K5" s="13">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="L5" s="14">
-        <v>9.249688112635894E-2</v>
+        <v>9.2625578909868181E-2</v>
       </c>
       <c r="M5" s="13">
         <v>85</v>
       </c>
       <c r="N5" s="16">
-        <v>1.321311985E-2</v>
+        <v>1.3211066210000001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="5">
+        <v>2020</v>
+      </c>
       <c r="C6" s="5">
         <v>12</v>
       </c>
@@ -706,25 +726,25 @@
         <v>45</v>
       </c>
       <c r="F6" s="7">
-        <v>0.54973681862788826</v>
+        <v>0.54978142564011068</v>
       </c>
       <c r="G6" s="7">
-        <v>0.45026318137211169</v>
+        <v>0.45021857435988938</v>
       </c>
       <c r="H6" s="8">
         <v>20210</v>
       </c>
       <c r="I6" s="9">
-        <v>3.8545274616526473E-2</v>
+        <v>3.8594755071746659E-2</v>
       </c>
       <c r="J6" s="8">
-        <v>19343</v>
+        <v>19344</v>
       </c>
       <c r="K6" s="8">
         <v>2204</v>
       </c>
       <c r="L6" s="7">
-        <v>0.11394302848575712</v>
+        <v>0.11393713813068652</v>
       </c>
       <c r="M6" s="6">
         <v>478</v>
@@ -734,26 +754,29 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="11">
+        <v>2020</v>
+      </c>
       <c r="C7" s="11">
         <v>13</v>
       </c>
       <c r="D7" s="12">
-        <v>34028</v>
+        <v>34029</v>
       </c>
       <c r="E7" s="13">
         <v>48</v>
       </c>
       <c r="F7" s="14">
-        <v>0.49494147403093935</v>
+        <v>0.49492691821309887</v>
       </c>
       <c r="G7" s="14">
-        <v>0.50505852596906065</v>
+        <v>0.50507308178690113</v>
       </c>
       <c r="H7" s="12">
-        <v>30858</v>
+        <v>30859</v>
       </c>
       <c r="I7" s="15">
-        <v>3.2438913733877764E-2</v>
+        <v>3.2470267993130041E-2</v>
       </c>
       <c r="J7" s="12">
         <v>29460</v>
@@ -765,13 +788,16 @@
         <v>0.17345553292600135</v>
       </c>
       <c r="M7" s="12">
-        <v>1457</v>
+        <v>1459</v>
       </c>
       <c r="N7" s="16">
-        <v>4.2817679550000001E-2</v>
+        <v>4.2875194679999999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="5">
+        <v>2020</v>
+      </c>
       <c r="C8" s="5">
         <v>14</v>
       </c>
@@ -782,86 +808,92 @@
         <v>51</v>
       </c>
       <c r="F8" s="7">
-        <v>0.45063937200077669</v>
+        <v>0.45066711048237218</v>
       </c>
       <c r="G8" s="7">
-        <v>0.54936062799922336</v>
+        <v>0.54933288951762782</v>
       </c>
       <c r="H8" s="8">
-        <v>31983</v>
+        <v>31984</v>
       </c>
       <c r="I8" s="9">
-        <v>5.3215770878279084E-2</v>
+        <v>5.3214107053526763E-2</v>
       </c>
       <c r="J8" s="8">
-        <v>31484</v>
+        <v>31485</v>
       </c>
       <c r="K8" s="8">
         <v>6064</v>
       </c>
       <c r="L8" s="7">
-        <v>0.1926057680091475</v>
+        <v>0.19259965062728282</v>
       </c>
       <c r="M8" s="8">
-        <v>2253</v>
+        <v>2254</v>
       </c>
       <c r="N8" s="10">
-        <v>6.2420346869999997E-2</v>
+        <v>6.2448052300000001E-2</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="11">
+        <v>2020</v>
+      </c>
       <c r="C9" s="11">
         <v>15</v>
       </c>
       <c r="D9" s="12">
-        <v>27188</v>
+        <v>27185</v>
       </c>
       <c r="E9" s="13">
         <v>52</v>
       </c>
       <c r="F9" s="14">
-        <v>0.43518791451731759</v>
+        <v>0.43516232450160297</v>
       </c>
       <c r="G9" s="14">
-        <v>0.56481208548268236</v>
+        <v>0.56483767549839703</v>
       </c>
       <c r="H9" s="12">
-        <v>23575</v>
+        <v>23574</v>
       </c>
       <c r="I9" s="15">
-        <v>8.3266171792152704E-2</v>
+        <v>8.3269703911088483E-2</v>
       </c>
       <c r="J9" s="12">
-        <v>24049</v>
+        <v>24047</v>
       </c>
       <c r="K9" s="12">
         <v>4710</v>
       </c>
       <c r="L9" s="14">
-        <v>0.19585013929893136</v>
+        <v>0.19586642824468747</v>
       </c>
       <c r="M9" s="12">
         <v>1870</v>
       </c>
       <c r="N9" s="16">
-        <v>6.8780344260000001E-2</v>
+        <v>6.8787934519999996E-2</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="5">
+        <v>2020</v>
+      </c>
       <c r="C10" s="5">
         <v>16</v>
       </c>
       <c r="D10" s="8">
-        <v>17363</v>
+        <v>17362</v>
       </c>
       <c r="E10" s="6">
         <v>51</v>
       </c>
       <c r="F10" s="7">
-        <v>0.44723183391003463</v>
+        <v>0.44728342369362095</v>
       </c>
       <c r="G10" s="7">
-        <v>0.55276816608996537</v>
+        <v>0.55271657630637905</v>
       </c>
       <c r="H10" s="8">
         <v>14861</v>
@@ -882,68 +914,74 @@
         <v>1212</v>
       </c>
       <c r="N10" s="10">
-        <v>6.9803605360000007E-2</v>
+        <v>6.9807625839999998E-2</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="11">
+        <v>2020</v>
+      </c>
       <c r="C11" s="11">
         <v>17</v>
       </c>
       <c r="D11" s="12">
-        <v>12381</v>
+        <v>12382</v>
       </c>
       <c r="E11" s="13">
         <v>50</v>
       </c>
       <c r="F11" s="14">
-        <v>0.44963184723683147</v>
+        <v>0.44967637540453076</v>
       </c>
       <c r="G11" s="14">
-        <v>0.55036815276316853</v>
+        <v>0.55032362459546924</v>
       </c>
       <c r="H11" s="12">
-        <v>10280</v>
+        <v>10282</v>
       </c>
       <c r="I11" s="15">
-        <v>0.13939688715953308</v>
+        <v>0.13936977241781753</v>
       </c>
       <c r="J11" s="12">
-        <v>10949</v>
+        <v>10950</v>
       </c>
       <c r="K11" s="12">
         <v>2225</v>
       </c>
       <c r="L11" s="14">
-        <v>0.20321490547081925</v>
+        <v>0.20319634703196346</v>
       </c>
       <c r="M11" s="13">
         <v>718</v>
       </c>
       <c r="N11" s="16">
-        <v>5.7992084639999997E-2</v>
+        <v>5.7987401059999999E-2</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="5">
+        <v>2020</v>
+      </c>
       <c r="C12" s="5">
         <v>18</v>
       </c>
       <c r="D12" s="8">
-        <v>7442</v>
+        <v>7443</v>
       </c>
       <c r="E12" s="6">
         <v>48</v>
       </c>
       <c r="F12" s="7">
-        <v>0.47814979158262738</v>
+        <v>0.47808550685668189</v>
       </c>
       <c r="G12" s="7">
-        <v>0.52185020841737262</v>
+        <v>0.52191449314331806</v>
       </c>
       <c r="H12" s="8">
-        <v>6243</v>
+        <v>6244</v>
       </c>
       <c r="I12" s="9">
-        <v>0.17683805862566074</v>
+        <v>0.17664958360025623</v>
       </c>
       <c r="J12" s="8">
         <v>6594</v>
@@ -955,13 +993,16 @@
         <v>0.20594479830148621</v>
       </c>
       <c r="M12" s="6">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="N12" s="10">
-        <v>5.1061542590000002E-2</v>
+        <v>5.118903667E-2</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="11">
+        <v>2020</v>
+      </c>
       <c r="C13" s="11">
         <v>19</v>
       </c>
@@ -1000,82 +1041,91 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="5">
+        <v>2020</v>
+      </c>
       <c r="C14" s="5">
         <v>20</v>
       </c>
       <c r="D14" s="8">
-        <v>4735</v>
+        <v>4734</v>
       </c>
       <c r="E14" s="6">
         <v>45</v>
       </c>
       <c r="F14" s="7">
-        <v>0.49407783417935702</v>
+        <v>0.49418235667442351</v>
       </c>
       <c r="G14" s="7">
-        <v>0.50592216582064298</v>
+        <v>0.50581764332557644</v>
       </c>
       <c r="H14" s="8">
-        <v>3936</v>
+        <v>3935</v>
       </c>
       <c r="I14" s="9">
-        <v>0.23272357723577236</v>
+        <v>0.23278271918678525</v>
       </c>
       <c r="J14" s="8">
-        <v>4206</v>
+        <v>4205</v>
       </c>
       <c r="K14" s="6">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="L14" s="7">
-        <v>0.17427484545886829</v>
+        <v>0.17455410225921522</v>
       </c>
       <c r="M14" s="6">
         <v>162</v>
       </c>
       <c r="N14" s="10">
-        <v>3.421330517E-2</v>
+        <v>3.4220532310000003E-2</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="11">
+        <v>2020</v>
+      </c>
       <c r="C15" s="11">
         <v>21</v>
       </c>
       <c r="D15" s="12">
-        <v>3617</v>
+        <v>3618</v>
       </c>
       <c r="E15" s="13">
         <v>43</v>
       </c>
       <c r="F15" s="14">
-        <v>0.50249861188228762</v>
+        <v>0.50263669164585068</v>
       </c>
       <c r="G15" s="14">
-        <v>0.49750138811771238</v>
+        <v>0.49736330835414932</v>
       </c>
       <c r="H15" s="12">
-        <v>2821</v>
+        <v>2822</v>
       </c>
       <c r="I15" s="15">
-        <v>0.26338177951081176</v>
+        <v>0.26293408929836998</v>
       </c>
       <c r="J15" s="12">
-        <v>3110</v>
+        <v>3111</v>
       </c>
       <c r="K15" s="13">
         <v>508</v>
       </c>
       <c r="L15" s="14">
-        <v>0.16334405144694533</v>
+        <v>0.16329154612664737</v>
       </c>
       <c r="M15" s="13">
         <v>109</v>
       </c>
       <c r="N15" s="16">
-        <v>3.0135471380000001E-2</v>
+        <v>3.0127142060000001E-2</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="5">
+        <v>2020</v>
+      </c>
       <c r="C16" s="5">
         <v>22</v>
       </c>
@@ -1113,7 +1163,10 @@
         <v>2.055434444E-2</v>
       </c>
     </row>
-    <row r="17" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="11">
+        <v>2020</v>
+      </c>
       <c r="C17" s="11">
         <v>23</v>
       </c>
@@ -1145,13 +1198,16 @@
         <v>0.148895292987512</v>
       </c>
       <c r="M17" s="13">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N17" s="16">
-        <v>1.906779661E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1.9491525419999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="5">
+        <v>2020</v>
+      </c>
       <c r="C18" s="5">
         <v>24</v>
       </c>
@@ -1168,10 +1224,10 @@
         <v>0.46358183376178236</v>
       </c>
       <c r="H18" s="8">
-        <v>1736</v>
+        <v>1737</v>
       </c>
       <c r="I18" s="9">
-        <v>0.24481566820276499</v>
+        <v>0.24467472654001152</v>
       </c>
       <c r="J18" s="8">
         <v>2085</v>
@@ -1189,12 +1245,15 @@
         <v>1.364605543E-2</v>
       </c>
     </row>
-    <row r="19" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="11">
+        <v>2020</v>
+      </c>
       <c r="C19" s="11">
         <v>25</v>
       </c>
       <c r="D19" s="12">
-        <v>4095</v>
+        <v>4096</v>
       </c>
       <c r="E19" s="13">
         <v>36</v>
@@ -1206,10 +1265,10 @@
         <v>0.41301688279911913</v>
       </c>
       <c r="H19" s="12">
-        <v>2937</v>
+        <v>2938</v>
       </c>
       <c r="I19" s="15">
-        <v>0.25059584610146407</v>
+        <v>0.25017018379850237</v>
       </c>
       <c r="J19" s="12">
         <v>3740</v>
@@ -1224,10 +1283,13 @@
         <v>38</v>
       </c>
       <c r="N19" s="16">
-        <v>9.2796092699999992E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>9.27734375E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="5">
+        <v>2020</v>
+      </c>
       <c r="C20" s="5">
         <v>26</v>
       </c>
@@ -1265,21 +1327,24 @@
         <v>7.1718116600000001E-3</v>
       </c>
     </row>
-    <row r="21" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="11">
+        <v>2020</v>
+      </c>
       <c r="C21" s="11">
         <v>27</v>
       </c>
       <c r="D21" s="12">
-        <v>2694</v>
+        <v>2695</v>
       </c>
       <c r="E21" s="13">
         <v>36</v>
       </c>
       <c r="F21" s="14">
-        <v>0.52209431860378763</v>
+        <v>0.52227171492204905</v>
       </c>
       <c r="G21" s="14">
-        <v>0.47790568139621242</v>
+        <v>0.47772828507795101</v>
       </c>
       <c r="H21" s="12">
         <v>2062</v>
@@ -1300,24 +1365,27 @@
         <v>26</v>
       </c>
       <c r="N21" s="16">
-        <v>9.6510764599999996E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>9.6474953599999993E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="5">
+        <v>2020</v>
+      </c>
       <c r="C22" s="5">
         <v>28</v>
       </c>
       <c r="D22" s="8">
-        <v>2425</v>
+        <v>2426</v>
       </c>
       <c r="E22" s="6">
         <v>36</v>
       </c>
       <c r="F22" s="7">
-        <v>0.55991735537190079</v>
+        <v>0.5596860801321768</v>
       </c>
       <c r="G22" s="7">
-        <v>0.44008264462809915</v>
+        <v>0.4403139198678232</v>
       </c>
       <c r="H22" s="8">
         <v>1923</v>
@@ -1326,22 +1394,25 @@
         <v>0.24024960998439937</v>
       </c>
       <c r="J22" s="8">
-        <v>2190</v>
+        <v>2191</v>
       </c>
       <c r="K22" s="6">
         <v>252</v>
       </c>
       <c r="L22" s="7">
-        <v>0.11506849315068493</v>
+        <v>0.11501597444089456</v>
       </c>
       <c r="M22" s="6">
         <v>25</v>
       </c>
       <c r="N22" s="10">
-        <v>1.0309278349999999E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1.030502885E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="11">
+        <v>2020</v>
+      </c>
       <c r="C23" s="11">
         <v>29</v>
       </c>
@@ -1379,45 +1450,51 @@
         <v>9.9206349199999991E-3</v>
       </c>
     </row>
-    <row r="24" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="5">
+        <v>2020</v>
+      </c>
       <c r="C24" s="5">
         <v>30</v>
       </c>
       <c r="D24" s="8">
-        <v>3938</v>
+        <v>3942</v>
       </c>
       <c r="E24" s="6">
         <v>36</v>
       </c>
       <c r="F24" s="7">
-        <v>0.52342158859470467</v>
+        <v>0.52339776195320442</v>
       </c>
       <c r="G24" s="7">
-        <v>0.47657841140529533</v>
+        <v>0.47660223804679552</v>
       </c>
       <c r="H24" s="8">
-        <v>3176</v>
+        <v>3178</v>
       </c>
       <c r="I24" s="9">
-        <v>0.27015113350125947</v>
+        <v>0.27029578351164252</v>
       </c>
       <c r="J24" s="8">
-        <v>3457</v>
+        <v>3460</v>
       </c>
       <c r="K24" s="6">
         <v>332</v>
       </c>
       <c r="L24" s="7">
-        <v>9.6037026323401789E-2</v>
+        <v>9.595375722543352E-2</v>
       </c>
       <c r="M24" s="6">
         <v>33</v>
       </c>
       <c r="N24" s="10">
-        <v>8.3798882599999992E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>8.37138508E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="11">
+        <v>2020</v>
+      </c>
       <c r="C25" s="11">
         <v>31</v>
       </c>
@@ -1443,10 +1520,10 @@
         <v>4129</v>
       </c>
       <c r="K25" s="13">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="L25" s="14">
-        <v>9.2758537176071687E-2</v>
+        <v>9.3000726568176317E-2</v>
       </c>
       <c r="M25" s="13">
         <v>32</v>
@@ -1455,7 +1532,10 @@
         <v>6.6334991700000004E-3</v>
       </c>
     </row>
-    <row r="26" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="5">
+        <v>2020</v>
+      </c>
       <c r="C26" s="5">
         <v>32</v>
       </c>
@@ -1466,25 +1546,25 @@
         <v>34</v>
       </c>
       <c r="F26" s="7">
-        <v>0.53685950413223138</v>
+        <v>0.53669421487603308</v>
       </c>
       <c r="G26" s="7">
-        <v>0.46314049586776862</v>
+        <v>0.46330578512396692</v>
       </c>
       <c r="H26" s="8">
-        <v>4531</v>
+        <v>4533</v>
       </c>
       <c r="I26" s="9">
-        <v>0.29949238578680204</v>
+        <v>0.29958085153320096</v>
       </c>
       <c r="J26" s="8">
-        <v>5264</v>
+        <v>5265</v>
       </c>
       <c r="K26" s="6">
         <v>398</v>
       </c>
       <c r="L26" s="7">
-        <v>7.560790273556231E-2</v>
+        <v>7.5593542260208924E-2</v>
       </c>
       <c r="M26" s="6">
         <v>30</v>
@@ -1493,27 +1573,30 @@
         <v>4.9480455200000004E-3</v>
       </c>
     </row>
-    <row r="27" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="11">
+        <v>2020</v>
+      </c>
       <c r="C27" s="11">
         <v>33</v>
       </c>
       <c r="D27" s="12">
-        <v>7956</v>
+        <v>7955</v>
       </c>
       <c r="E27" s="13">
         <v>32</v>
       </c>
       <c r="F27" s="14">
-        <v>0.53318221886412287</v>
+        <v>0.53324937027707808</v>
       </c>
       <c r="G27" s="14">
-        <v>0.46681778113587707</v>
+        <v>0.46675062972292192</v>
       </c>
       <c r="H27" s="12">
-        <v>5813</v>
+        <v>5812</v>
       </c>
       <c r="I27" s="15">
-        <v>0.33184242215723381</v>
+        <v>0.33189951823812802</v>
       </c>
       <c r="J27" s="12">
         <v>6966</v>
@@ -1528,733 +1611,830 @@
         <v>30</v>
       </c>
       <c r="N27" s="16">
-        <v>3.7707390600000001E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>3.77121307E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="5">
+        <v>2020</v>
+      </c>
       <c r="C28" s="5">
         <v>34</v>
       </c>
       <c r="D28" s="8">
-        <v>9587</v>
+        <v>9603</v>
       </c>
       <c r="E28" s="6">
         <v>32</v>
       </c>
       <c r="F28" s="7">
-        <v>0.54744908671005665</v>
+        <v>0.54768392370572205</v>
       </c>
       <c r="G28" s="7">
-        <v>0.45255091328994329</v>
+        <v>0.45231607629427795</v>
       </c>
       <c r="H28" s="8">
-        <v>7161</v>
+        <v>7165</v>
       </c>
       <c r="I28" s="9">
-        <v>0.34464460270911884</v>
+        <v>0.34445219818562456</v>
       </c>
       <c r="J28" s="8">
-        <v>8232</v>
+        <v>8238</v>
       </c>
       <c r="K28" s="6">
         <v>429</v>
       </c>
       <c r="L28" s="7">
-        <v>5.2113702623906709E-2</v>
+        <v>5.2075746540422435E-2</v>
       </c>
       <c r="M28" s="6">
         <v>30</v>
       </c>
       <c r="N28" s="10">
-        <v>3.1292375000000002E-3</v>
-      </c>
-    </row>
-    <row r="29" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>3.1240237400000002E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="11">
+        <v>2020</v>
+      </c>
       <c r="C29" s="11">
         <v>35</v>
       </c>
       <c r="D29" s="12">
-        <v>8819</v>
+        <v>8821</v>
       </c>
       <c r="E29" s="13">
         <v>32</v>
       </c>
       <c r="F29" s="14">
-        <v>0.53020440790224965</v>
+        <v>0.53019751113140767</v>
       </c>
       <c r="G29" s="14">
-        <v>0.46979559209775035</v>
+        <v>0.46980248886859233</v>
       </c>
       <c r="H29" s="12">
-        <v>6828</v>
+        <v>6834</v>
       </c>
       <c r="I29" s="15">
-        <v>0.30726420620972467</v>
+        <v>0.307140766754463</v>
       </c>
       <c r="J29" s="12">
-        <v>7337</v>
+        <v>7344</v>
       </c>
       <c r="K29" s="13">
         <v>364</v>
       </c>
       <c r="L29" s="14">
-        <v>4.9611557857434922E-2</v>
+        <v>4.9564270152505446E-2</v>
       </c>
       <c r="M29" s="13">
         <v>20</v>
       </c>
       <c r="N29" s="16">
-        <v>2.26783081E-3</v>
-      </c>
-    </row>
-    <row r="30" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.2673166300000002E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="5">
+        <v>2020</v>
+      </c>
       <c r="C30" s="5">
         <v>36</v>
       </c>
       <c r="D30" s="8">
-        <v>8616</v>
+        <v>8619</v>
       </c>
       <c r="E30" s="6">
         <v>33</v>
       </c>
       <c r="F30" s="7">
-        <v>0.53658536585365857</v>
+        <v>0.53651423238450768</v>
       </c>
       <c r="G30" s="7">
-        <v>0.46341463414634149</v>
+        <v>0.46348576761549232</v>
       </c>
       <c r="H30" s="8">
-        <v>6574</v>
+        <v>6601</v>
       </c>
       <c r="I30" s="9">
-        <v>0.26969881350775782</v>
+        <v>0.26844417512498109</v>
       </c>
       <c r="J30" s="8">
-        <v>6981</v>
+        <v>7007</v>
       </c>
       <c r="K30" s="6">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="L30" s="7">
-        <v>5.6152413694313133E-2</v>
+        <v>5.6372199229342085E-2</v>
       </c>
       <c r="M30" s="6">
         <v>36</v>
       </c>
       <c r="N30" s="10">
-        <v>4.1782729799999998E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>4.1768186499999997E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="11">
+        <v>2020</v>
+      </c>
       <c r="C31" s="11">
         <v>37</v>
       </c>
       <c r="D31" s="12">
-        <v>9766</v>
+        <v>9767</v>
       </c>
       <c r="E31" s="13">
         <v>35</v>
       </c>
       <c r="F31" s="14">
-        <v>0.51884654994850665</v>
+        <v>0.51899907321594063</v>
       </c>
       <c r="G31" s="14">
-        <v>0.48115345005149329</v>
+        <v>0.48100092678405931</v>
       </c>
       <c r="H31" s="12">
-        <v>7487</v>
+        <v>7527</v>
       </c>
       <c r="I31" s="15">
-        <v>0.20488847335381327</v>
+        <v>0.20273681413577788</v>
       </c>
       <c r="J31" s="12">
-        <v>7877</v>
+        <v>7938</v>
       </c>
       <c r="K31" s="13">
-        <v>458</v>
+        <v>463</v>
       </c>
       <c r="L31" s="14">
-        <v>5.8143963437857049E-2</v>
+        <v>5.8327034517510708E-2</v>
       </c>
       <c r="M31" s="13">
         <v>62</v>
       </c>
       <c r="N31" s="16">
-        <v>6.34855621E-3</v>
-      </c>
-    </row>
-    <row r="32" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>6.3479062100000004E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="5">
+        <v>2020</v>
+      </c>
       <c r="C32" s="5">
         <v>38</v>
       </c>
       <c r="D32" s="8">
-        <v>12278</v>
+        <v>12279</v>
       </c>
       <c r="E32" s="6">
         <v>36</v>
       </c>
       <c r="F32" s="7">
-        <v>0.51162790697674421</v>
+        <v>0.5115860149021535</v>
       </c>
       <c r="G32" s="7">
-        <v>0.48837209302325579</v>
+        <v>0.48841398509784656</v>
       </c>
       <c r="H32" s="8">
-        <v>9555</v>
+        <v>9590</v>
       </c>
       <c r="I32" s="9">
-        <v>0.1870225013082156</v>
+        <v>0.18633993743482793</v>
       </c>
       <c r="J32" s="8">
-        <v>9876</v>
+        <v>9929</v>
       </c>
       <c r="K32" s="6">
-        <v>656</v>
+        <v>660</v>
       </c>
       <c r="L32" s="7">
-        <v>6.6423653300931557E-2</v>
+        <v>6.6471950851042405E-2</v>
       </c>
       <c r="M32" s="6">
         <v>78</v>
       </c>
       <c r="N32" s="10">
-        <v>6.3528261899999999E-3</v>
-      </c>
-    </row>
-    <row r="33" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>6.3523088100000003E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="11">
+        <v>2020</v>
+      </c>
       <c r="C33" s="11">
         <v>39</v>
       </c>
       <c r="D33" s="12">
-        <v>13058</v>
+        <v>13070</v>
       </c>
       <c r="E33" s="13">
         <v>37</v>
       </c>
       <c r="F33" s="14">
-        <v>0.51609177702494613</v>
+        <v>0.51623076923076927</v>
       </c>
       <c r="G33" s="14">
-        <v>0.48390822297505387</v>
+        <v>0.48376923076923078</v>
       </c>
       <c r="H33" s="12">
-        <v>10182</v>
+        <v>10216</v>
       </c>
       <c r="I33" s="15">
-        <v>0.184639560007857</v>
+        <v>0.18382928739232576</v>
       </c>
       <c r="J33" s="12">
-        <v>10656</v>
+        <v>10686</v>
       </c>
       <c r="K33" s="13">
-        <v>750</v>
+        <v>754</v>
       </c>
       <c r="L33" s="14">
-        <v>7.0382882882882886E-2</v>
+        <v>7.0559610705596104E-2</v>
       </c>
       <c r="M33" s="13">
         <v>106</v>
       </c>
       <c r="N33" s="16">
-        <v>8.1176290300000002E-3</v>
-      </c>
-    </row>
-    <row r="34" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>8.1101759699999994E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="5">
+        <v>2020</v>
+      </c>
       <c r="C34" s="5">
         <v>40</v>
       </c>
       <c r="D34" s="8">
-        <v>15914</v>
+        <v>15920</v>
       </c>
       <c r="E34" s="6">
         <v>38</v>
       </c>
       <c r="F34" s="7">
-        <v>0.51970738475121403</v>
+        <v>0.51969993065624409</v>
       </c>
       <c r="G34" s="7">
-        <v>0.48029261524878603</v>
+        <v>0.48030006934375591</v>
       </c>
       <c r="H34" s="8">
-        <v>12235</v>
+        <v>12308</v>
       </c>
       <c r="I34" s="9">
-        <v>0.174989783408255</v>
+        <v>0.17541436464088397</v>
       </c>
       <c r="J34" s="8">
-        <v>13172</v>
+        <v>13214</v>
       </c>
       <c r="K34" s="6">
-        <v>854</v>
+        <v>858</v>
       </c>
       <c r="L34" s="7">
-        <v>6.4834497418767081E-2</v>
+        <v>6.4931133646132885E-2</v>
       </c>
       <c r="M34" s="6">
         <v>119</v>
       </c>
       <c r="N34" s="10">
-        <v>7.4776925899999996E-3</v>
-      </c>
-    </row>
-    <row r="35" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>7.4748743699999997E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="17">
+        <v>2020</v>
+      </c>
       <c r="C35" s="17">
         <v>41</v>
       </c>
       <c r="D35" s="18">
-        <v>26158</v>
+        <v>26164</v>
       </c>
       <c r="E35" s="19">
         <v>39</v>
       </c>
       <c r="F35" s="20">
-        <v>0.51035224522721157</v>
+        <v>0.51031145589308347</v>
       </c>
       <c r="G35" s="20">
-        <v>0.48964775477278838</v>
+        <v>0.48968854410691653</v>
       </c>
       <c r="H35" s="18">
-        <v>19292</v>
+        <v>19329</v>
       </c>
       <c r="I35" s="21">
-        <v>0.16483516483516483</v>
+        <v>0.16514046251746081</v>
       </c>
       <c r="J35" s="18">
-        <v>20930</v>
+        <v>20955</v>
       </c>
       <c r="K35" s="19">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="L35" s="20">
-        <v>7.2718585762064025E-2</v>
+        <v>7.2679551419708902E-2</v>
       </c>
       <c r="M35" s="19">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="N35" s="22">
-        <v>8.7162627100000004E-3</v>
-      </c>
-    </row>
-    <row r="36" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>8.7907047800000002E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="5">
+        <v>2020</v>
+      </c>
       <c r="C36" s="5">
         <v>42</v>
       </c>
       <c r="D36" s="8">
-        <v>42068</v>
+        <v>42069</v>
       </c>
       <c r="E36" s="6">
         <v>39</v>
       </c>
       <c r="F36" s="7">
-        <v>0.5085650031101967</v>
+        <v>0.50852891217493246</v>
       </c>
       <c r="G36" s="7">
-        <v>0.49143499688980335</v>
+        <v>0.4914710878250676</v>
       </c>
       <c r="H36" s="8">
-        <v>29335</v>
+        <v>29373</v>
       </c>
       <c r="I36" s="9">
-        <v>0.15844554286688256</v>
+        <v>0.15844483028631737</v>
       </c>
       <c r="J36" s="8">
-        <v>32432</v>
+        <v>32448</v>
       </c>
       <c r="K36" s="6">
-        <v>2223</v>
+        <v>2224</v>
       </c>
       <c r="L36" s="7">
-        <v>6.8543413912185491E-2</v>
+        <v>6.8540433925049313E-2</v>
       </c>
       <c r="M36" s="6">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N36" s="10">
-        <v>1.0364172289999999E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1.03876964E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="17">
+        <v>2020</v>
+      </c>
       <c r="C37" s="17">
         <v>43</v>
       </c>
       <c r="D37" s="12">
-        <v>74826</v>
+        <v>74835</v>
       </c>
       <c r="E37" s="13">
         <v>40</v>
       </c>
       <c r="F37" s="14">
-        <v>0.50192987882781714</v>
+        <v>0.50186233511274858</v>
       </c>
       <c r="G37" s="14">
-        <v>0.49807012117218286</v>
+        <v>0.49813766488725142</v>
       </c>
       <c r="H37" s="12">
-        <v>47816</v>
+        <v>48165</v>
       </c>
       <c r="I37" s="15">
-        <v>0.15365149740672579</v>
+        <v>0.15357624831309041</v>
       </c>
       <c r="J37" s="12">
-        <v>54399</v>
+        <v>54686</v>
       </c>
       <c r="K37" s="13">
-        <v>3832</v>
+        <v>3857</v>
       </c>
       <c r="L37" s="14">
-        <v>7.0442471368958995E-2</v>
+        <v>7.0529934535347255E-2</v>
       </c>
       <c r="M37" s="13">
-        <v>917</v>
+        <v>924</v>
       </c>
       <c r="N37" s="16">
-        <v>1.225509849E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1.234716376E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="5">
+        <v>2020</v>
+      </c>
       <c r="C38" s="5">
         <v>44</v>
       </c>
       <c r="D38" s="8">
-        <v>111161</v>
+        <v>111149</v>
       </c>
       <c r="E38" s="6">
         <v>41</v>
       </c>
       <c r="F38" s="7">
-        <v>0.49724328049620953</v>
+        <v>0.49723401168063264</v>
       </c>
       <c r="G38" s="7">
-        <v>0.50275671950379053</v>
+        <v>0.50276598831936736</v>
       </c>
       <c r="H38" s="8">
-        <v>67643</v>
+        <v>68766</v>
       </c>
       <c r="I38" s="9">
-        <v>0.15499016897535592</v>
+        <v>0.15577465608003954</v>
       </c>
       <c r="J38" s="8">
-        <v>77867</v>
+        <v>78570</v>
       </c>
       <c r="K38" s="6">
-        <v>5444</v>
+        <v>5512</v>
       </c>
       <c r="L38" s="7">
-        <v>6.9914084271899518E-2</v>
+        <v>7.0154002800050907E-2</v>
       </c>
       <c r="M38" s="6">
-        <v>1455</v>
+        <v>1467</v>
       </c>
       <c r="N38" s="10">
-        <v>1.3089122979999999E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1.319849931E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="17">
+        <v>2020</v>
+      </c>
       <c r="C39" s="17">
         <v>45</v>
       </c>
       <c r="D39" s="18">
-        <v>125775</v>
+        <v>125794</v>
       </c>
       <c r="E39" s="19">
         <v>41</v>
       </c>
       <c r="F39" s="20">
-        <v>0.49124342554302003</v>
+        <v>0.49130567419158022</v>
       </c>
       <c r="G39" s="20">
-        <v>0.50875657445697997</v>
+        <v>0.50869432580841978</v>
       </c>
       <c r="H39" s="18">
-        <v>73811</v>
+        <v>74342</v>
       </c>
       <c r="I39" s="21">
-        <v>0.14871767080787415</v>
+        <v>0.14883914879879476</v>
       </c>
       <c r="J39" s="18">
-        <v>84191</v>
+        <v>84517</v>
       </c>
       <c r="K39" s="19">
-        <v>6121</v>
+        <v>6163</v>
       </c>
       <c r="L39" s="20">
-        <v>7.2703733178130683E-2</v>
+        <v>7.2920240898280822E-2</v>
       </c>
       <c r="M39" s="19">
-        <v>1659</v>
+        <v>1684</v>
       </c>
       <c r="N39" s="22">
-        <v>1.3190220630000001E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1.3386965989999999E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="5">
+        <v>2020</v>
+      </c>
       <c r="C40" s="5">
         <v>46</v>
       </c>
       <c r="D40" s="8">
-        <v>127842</v>
+        <v>127875</v>
       </c>
       <c r="E40" s="6">
         <v>42</v>
       </c>
       <c r="F40" s="7">
-        <v>0.48466369273601617</v>
+        <v>0.48459281867997184</v>
       </c>
       <c r="G40" s="7">
-        <v>0.51533630726398383</v>
+        <v>0.51540718132002816</v>
       </c>
       <c r="H40" s="8">
-        <v>74502</v>
+        <v>74878</v>
       </c>
       <c r="I40" s="9">
-        <v>0.14669404848191994</v>
+        <v>0.14671866235743475</v>
       </c>
       <c r="J40" s="8">
-        <v>85313</v>
+        <v>85689</v>
       </c>
       <c r="K40" s="6">
-        <v>6648</v>
+        <v>6690</v>
       </c>
       <c r="L40" s="7">
-        <v>7.7924818023044559E-2</v>
+        <v>7.8073031544305574E-2</v>
       </c>
       <c r="M40" s="6">
-        <v>2164</v>
+        <v>2197</v>
       </c>
       <c r="N40" s="10">
-        <v>1.692714444E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1.7180840659999998E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="17">
+        <v>2020</v>
+      </c>
       <c r="C41" s="17">
         <v>47</v>
       </c>
       <c r="D41" s="18">
-        <v>128532</v>
+        <v>128528</v>
       </c>
       <c r="E41" s="19">
         <v>43</v>
       </c>
       <c r="F41" s="20">
-        <v>0.47459462853375611</v>
+        <v>0.47457108324046021</v>
       </c>
       <c r="G41" s="20">
-        <v>0.52540537146624389</v>
+        <v>0.52542891675953973</v>
       </c>
       <c r="H41" s="18">
-        <v>75458</v>
+        <v>75998</v>
       </c>
       <c r="I41" s="21">
-        <v>0.1472607278220997</v>
+        <v>0.14699071028184951</v>
       </c>
       <c r="J41" s="18">
-        <v>84886</v>
+        <v>85457</v>
       </c>
       <c r="K41" s="19">
-        <v>7088</v>
+        <v>7158</v>
       </c>
       <c r="L41" s="20">
-        <v>8.3500223829606771E-2</v>
+        <v>8.3761423873995114E-2</v>
       </c>
       <c r="M41" s="19">
-        <v>2620</v>
+        <v>2729</v>
       </c>
       <c r="N41" s="22">
-        <v>2.0384028870000001E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.1232727489999999E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="5">
+        <v>2020</v>
+      </c>
       <c r="C42" s="5">
         <v>48</v>
       </c>
       <c r="D42" s="8">
-        <v>123357</v>
+        <v>123370</v>
       </c>
       <c r="E42" s="6">
         <v>44</v>
       </c>
       <c r="F42" s="7">
-        <v>0.46568478963871401</v>
+        <v>0.46567953377205906</v>
       </c>
       <c r="G42" s="7">
-        <v>0.53431521036128604</v>
+        <v>0.53432046622794094</v>
       </c>
       <c r="H42" s="8">
-        <v>70830</v>
+        <v>71397</v>
       </c>
       <c r="I42" s="9">
-        <v>0.1540590145418608</v>
+        <v>0.1535078504699077</v>
       </c>
       <c r="J42" s="8">
-        <v>80434</v>
+        <v>81099</v>
       </c>
       <c r="K42" s="6">
-        <v>7181</v>
+        <v>7266</v>
       </c>
       <c r="L42" s="7">
-        <v>8.9278165949722751E-2</v>
+        <v>8.959419968187031E-2</v>
       </c>
       <c r="M42" s="6">
-        <v>2728</v>
+        <v>2845</v>
       </c>
       <c r="N42" s="10">
-        <v>2.211467529E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.3060711679999998E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="17">
+        <v>2020</v>
+      </c>
       <c r="C43" s="17">
         <v>49</v>
       </c>
       <c r="D43" s="18">
-        <v>128304</v>
+        <v>128337</v>
       </c>
       <c r="E43" s="19">
         <v>45</v>
       </c>
       <c r="F43" s="20">
-        <v>0.45960529524199067</v>
+        <v>0.45946243492757499</v>
       </c>
       <c r="G43" s="20">
-        <v>0.54039470475800933</v>
+        <v>0.54053756507242501</v>
       </c>
       <c r="H43" s="18">
-        <v>73303</v>
+        <v>74347</v>
       </c>
       <c r="I43" s="21">
-        <v>0.14385495818725019</v>
+        <v>0.14371797113535179</v>
       </c>
       <c r="J43" s="18">
-        <v>82678</v>
+        <v>83590</v>
       </c>
       <c r="K43" s="19">
-        <v>7620</v>
+        <v>7774</v>
       </c>
       <c r="L43" s="20">
-        <v>9.2164783860277225E-2</v>
+        <v>9.3001555209953346E-2</v>
       </c>
       <c r="M43" s="19">
-        <v>2956</v>
+        <v>3252</v>
       </c>
       <c r="N43" s="22">
-        <v>2.3039032290000001E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.5339535749999999E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="5">
+        <v>2020</v>
+      </c>
       <c r="C44" s="5">
         <v>50</v>
       </c>
       <c r="D44" s="8">
-        <v>155956</v>
+        <v>156115</v>
       </c>
       <c r="E44" s="6">
         <v>46</v>
       </c>
       <c r="F44" s="7">
-        <v>0.45375073604110183</v>
+        <v>0.45373931140569151</v>
       </c>
       <c r="G44" s="7">
-        <v>0.54624926395889817</v>
+        <v>0.54626068859430843</v>
       </c>
       <c r="H44" s="8">
-        <v>86334</v>
+        <v>88394</v>
       </c>
       <c r="I44" s="9">
-        <v>0.14894479579308267</v>
+        <v>0.14822273004955089</v>
       </c>
       <c r="J44" s="8">
-        <v>97363</v>
+        <v>99388</v>
       </c>
       <c r="K44" s="6">
-        <v>8883</v>
+        <v>9283</v>
       </c>
       <c r="L44" s="7">
-        <v>9.1235890430656413E-2</v>
+        <v>9.3401617901557529E-2</v>
       </c>
       <c r="M44" s="6">
-        <v>3064</v>
+        <v>3770</v>
       </c>
       <c r="N44" s="10">
-        <v>1.9646566979999999E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.4148864610000001E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="17">
+        <v>2020</v>
+      </c>
       <c r="C45" s="17">
         <v>51</v>
       </c>
       <c r="D45" s="18">
-        <v>173481</v>
+        <v>174066</v>
       </c>
       <c r="E45" s="19">
         <v>46</v>
       </c>
       <c r="F45" s="20">
-        <v>0.45225701007962499</v>
+        <v>0.45204399782097199</v>
       </c>
       <c r="G45" s="20">
-        <v>0.54774298992037507</v>
+        <v>0.54795600217902807</v>
       </c>
       <c r="H45" s="18">
-        <v>89081</v>
+        <v>92973</v>
       </c>
       <c r="I45" s="21">
-        <v>0.14788787732513106</v>
+        <v>0.14763425940864552</v>
       </c>
       <c r="J45" s="18">
-        <v>101764</v>
+        <v>105501</v>
       </c>
       <c r="K45" s="19">
-        <v>8899</v>
+        <v>9792</v>
       </c>
       <c r="L45" s="20">
-        <v>8.7447427380999171E-2</v>
+        <v>9.2814286120510708E-2</v>
       </c>
       <c r="M45" s="19">
-        <v>2118</v>
+        <v>3367</v>
       </c>
       <c r="N45" s="22">
-        <v>1.220882978E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1.9343237619999998E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="5">
+        <v>2020</v>
+      </c>
       <c r="C46" s="5">
         <v>52</v>
       </c>
       <c r="D46" s="8">
-        <v>135974</v>
+        <v>138246</v>
       </c>
       <c r="E46" s="6">
         <v>48</v>
       </c>
       <c r="F46" s="7">
-        <v>0.44564085784824059</v>
+        <v>0.44503443792773512</v>
       </c>
       <c r="G46" s="7">
-        <v>0.55435914215175941</v>
+        <v>0.55496556207226488</v>
       </c>
       <c r="H46" s="8">
-        <v>56966</v>
+        <v>68033</v>
       </c>
       <c r="I46" s="9">
-        <v>0.16200891759997191</v>
+        <v>0.15630649831699323</v>
       </c>
       <c r="J46" s="8">
-        <v>71416</v>
+        <v>80723</v>
       </c>
       <c r="K46" s="6">
-        <v>5983</v>
+        <v>7682</v>
       </c>
       <c r="L46" s="7">
-        <v>8.3776744707068446E-2</v>
+        <v>9.5164946793355049E-2</v>
       </c>
       <c r="M46" s="6">
-        <v>732</v>
+        <v>1895</v>
       </c>
       <c r="N46" s="10">
-        <v>5.3833821100000004E-3</v>
+        <v>1.370744904E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="17">
+        <v>2020</v>
+      </c>
+      <c r="C47" s="17">
+        <v>53</v>
+      </c>
+      <c r="D47" s="18">
+        <v>120472</v>
+      </c>
+      <c r="E47" s="19">
+        <v>49</v>
+      </c>
+      <c r="F47" s="20">
+        <v>0.44145135151021503</v>
+      </c>
+      <c r="G47" s="20">
+        <v>0.55854864848978492</v>
+      </c>
+      <c r="H47" s="18">
+        <v>53848</v>
+      </c>
+      <c r="I47" s="21">
+        <v>0.13584534244540186</v>
+      </c>
+      <c r="J47" s="18">
+        <v>66197</v>
+      </c>
+      <c r="K47" s="19">
+        <v>6128</v>
+      </c>
+      <c r="L47" s="20">
+        <v>9.2572170944302618E-2</v>
+      </c>
+      <c r="M47" s="19">
+        <v>837</v>
+      </c>
+      <c r="N47" s="22">
+        <v>6.94767248E-3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update corona report table
</commit_message>
<xml_diff>
--- a/data/klinische_aspekte.xlsx
+++ b/data/klinische_aspekte.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B99830-1146-4F2B-B351-A2F8CCC330C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5EE099-23AD-46C4-8872-4CAFBB78C315}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1" xr2:uid="{3677AF26-2CAB-4FDE-A93C-D8C0E4111944}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6936" activeTab="2" xr2:uid="{3677AF26-2CAB-4FDE-A93C-D8C0E4111944}"/>
   </bookViews>
   <sheets>
     <sheet name="Klinische_Aspekte" sheetId="2" r:id="rId1"/>
     <sheet name="Fälle_Hospitalisierung_Alter" sheetId="1" r:id="rId2"/>
+    <sheet name="Alter_Median_Mittelwert" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="106">
   <si>
     <t>Meldejahr</t>
   </si>
@@ -312,16 +313,44 @@
   </si>
   <si>
     <t>2021-KW17</t>
+  </si>
+  <si>
+    <t>Altersmedian alle COVID-19-Fälle</t>
+  </si>
+  <si>
+    <t>Altersmedian hospitalisierte Fälle</t>
+  </si>
+  <si>
+    <t>Altersmedian der Fälle auf Intensivstation</t>
+  </si>
+  <si>
+    <t>Altersmedian der verstorbenen COVID-19-Fälle</t>
+  </si>
+  <si>
+    <t>Anzahl COVID-19-Fälle</t>
+  </si>
+  <si>
+    <t>Mittelwert Alter alle COVID-19-Fälle</t>
+  </si>
+  <si>
+    <t>Mittelwert Alter hospitalisierte Fälle</t>
+  </si>
+  <si>
+    <t>Mittelwert Alter  Fälle auf Intensivstation</t>
+  </si>
+  <si>
+    <t>Mittelwert Alter der verstorbenen COVID-19-Fälle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,6 +375,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -396,7 +431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -500,6 +535,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -817,18 +862,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{872BAA18-906B-41C7-A8B5-537096EA6980}">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="60" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -869,7 +914,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2020</v>
       </c>
@@ -910,7 +955,7 @@
         <v>1.337792642E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11">
         <v>2020</v>
       </c>
@@ -951,7 +996,7 @@
         <v>1.306579561E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17">
         <v>2020</v>
       </c>
@@ -992,7 +1037,7 @@
         <v>2.1153159580000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11">
         <v>2020</v>
       </c>
@@ -1033,7 +1078,7 @@
         <v>4.2979099200000002E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="17">
         <v>2020</v>
       </c>
@@ -1074,7 +1119,7 @@
         <v>6.2631754129999995E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11">
         <v>2020</v>
       </c>
@@ -1115,7 +1160,7 @@
         <v>6.9082339069999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="17">
         <v>2020</v>
       </c>
@@ -1156,7 +1201,7 @@
         <v>7.0176450230000006E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11">
         <v>2020</v>
       </c>
@@ -1197,7 +1242,7 @@
         <v>5.8499878630000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="17">
         <v>2020</v>
       </c>
@@ -1238,7 +1283,7 @@
         <v>5.1895670870000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11">
         <v>2020</v>
       </c>
@@ -1279,7 +1324,7 @@
         <v>4.1192498789999997E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="17">
         <v>2020</v>
       </c>
@@ -1320,7 +1365,7 @@
         <v>3.4446544840000003E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="11">
         <v>2020</v>
       </c>
@@ -1361,7 +1406,7 @@
         <v>3.1380172169999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="17">
         <v>2020</v>
       </c>
@@ -1402,7 +1447,7 @@
         <v>2.026816339E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11">
         <v>2020</v>
       </c>
@@ -1443,7 +1488,7 @@
         <v>1.9140791149999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="17">
         <v>2020</v>
       </c>
@@ -1484,7 +1529,7 @@
         <v>1.409052092E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11">
         <v>2020</v>
       </c>
@@ -1525,7 +1570,7 @@
         <v>9.9369849699999999E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="17">
         <v>2020</v>
       </c>
@@ -1566,7 +1611,7 @@
         <v>7.1628776E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11">
         <v>2020</v>
       </c>
@@ -1607,7 +1652,7 @@
         <v>9.6654275000000005E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="17">
         <v>2020</v>
       </c>
@@ -1648,7 +1693,7 @@
         <v>1.030502885E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11">
         <v>2020</v>
       </c>
@@ -1689,7 +1734,7 @@
         <v>9.9469495999999994E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="17">
         <v>2020</v>
       </c>
@@ -1730,7 +1775,7 @@
         <v>8.3990837299999996E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11">
         <v>2020</v>
       </c>
@@ -1771,7 +1816,7 @@
         <v>6.6348745500000002E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="17">
         <v>2020</v>
       </c>
@@ -1812,7 +1857,7 @@
         <v>5.1205814299999999E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11">
         <v>2020</v>
       </c>
@@ -1853,7 +1898,7 @@
         <v>3.7740596299999998E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="17">
         <v>2020</v>
       </c>
@@ -1894,7 +1939,7 @@
         <v>3.12793243E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="11">
         <v>2020</v>
       </c>
@@ -1935,7 +1980,7 @@
         <v>2.04081632E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="17">
         <v>2020</v>
       </c>
@@ -1976,7 +2021,7 @@
         <v>4.1787579800000004E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="11">
         <v>2020</v>
       </c>
@@ -2017,7 +2062,7 @@
         <v>6.7567567499999997E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="17">
         <v>2020</v>
       </c>
@@ -2058,7 +2103,7 @@
         <v>6.5072393000000003E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="11">
         <v>2020</v>
       </c>
@@ -2099,7 +2144,7 @@
         <v>8.1904470300000008E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="17">
         <v>2020</v>
       </c>
@@ -2140,7 +2185,7 @@
         <v>7.5966850800000003E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="18">
         <v>2020</v>
       </c>
@@ -2181,7 +2226,7 @@
         <v>9.1479751899999993E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="17">
         <v>2020</v>
       </c>
@@ -2222,7 +2267,7 @@
         <v>1.0906239599999999E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="18">
         <v>2020</v>
       </c>
@@ -2263,7 +2308,7 @@
         <v>1.324671505E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="17">
         <v>2020</v>
       </c>
@@ -2304,7 +2349,7 @@
         <v>1.433227101E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="18">
         <v>2020</v>
       </c>
@@ -2345,7 +2390,7 @@
         <v>1.4770179810000001E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="17">
         <v>2020</v>
       </c>
@@ -2386,7 +2431,7 @@
         <v>1.931335507E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="18">
         <v>2020</v>
       </c>
@@ -2427,7 +2472,7 @@
         <v>2.4524115379999999E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="17">
         <v>2020</v>
       </c>
@@ -2468,7 +2513,7 @@
         <v>2.846992408E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="18">
         <v>2020</v>
       </c>
@@ -2509,7 +2554,7 @@
         <v>3.402625905E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="17">
         <v>2020</v>
       </c>
@@ -2550,7 +2595,7 @@
         <v>3.5810823759999999E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="18">
         <v>2020</v>
       </c>
@@ -2591,7 +2636,7 @@
         <v>3.5899107380000003E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="17">
         <v>2020</v>
       </c>
@@ -2632,7 +2677,7 @@
         <v>4.0006036469999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="18">
         <v>2020</v>
       </c>
@@ -2673,7 +2718,7 @@
         <v>4.5058505409999998E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="25">
         <v>2021</v>
       </c>
@@ -2714,7 +2759,7 @@
         <v>3.8066967620000003E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="18">
         <v>2021</v>
       </c>
@@ -2755,7 +2800,7 @@
         <v>4.1461919040000003E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="17">
         <v>2021</v>
       </c>
@@ -2796,7 +2841,7 @@
         <v>4.1087006539999998E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="18">
         <v>2021</v>
       </c>
@@ -2837,7 +2882,7 @@
         <v>3.8198083059999999E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="17">
         <v>2021</v>
       </c>
@@ -2878,7 +2923,7 @@
         <v>3.3137979550000002E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="18">
         <v>2021</v>
       </c>
@@ -2919,7 +2964,7 @@
         <v>3.169422543E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="17">
         <v>2021</v>
       </c>
@@ -2960,7 +3005,7 @@
         <v>2.6652187989999999E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="18">
         <v>2021</v>
       </c>
@@ -3001,7 +3046,7 @@
         <v>2.030115146E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="17">
         <v>2021</v>
       </c>
@@ -3042,7 +3087,7 @@
         <v>1.6307692299999999E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="18">
         <v>2021</v>
       </c>
@@ -3083,7 +3128,7 @@
         <v>1.392465293E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="17">
         <v>2021</v>
       </c>
@@ -3124,7 +3169,7 @@
         <v>1.2201562920000001E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="18">
         <v>2021</v>
       </c>
@@ -3165,7 +3210,7 @@
         <v>1.122680023E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="17">
         <v>2021</v>
       </c>
@@ -3206,7 +3251,7 @@
         <v>1.1294676010000001E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="18">
         <v>2021</v>
       </c>
@@ -3247,7 +3292,7 @@
         <v>9.2137125600000001E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="17">
         <v>2021</v>
       </c>
@@ -3288,7 +3333,7 @@
         <v>6.5662092699999997E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="18">
         <v>2021</v>
       </c>
@@ -3329,7 +3374,7 @@
         <v>3.64672207E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="25">
         <v>2021</v>
       </c>
@@ -3372,7 +3417,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3380,19 +3425,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29EE44EF-F204-44BC-9DFD-46318AB81991}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="33"/>
-    <col min="2" max="2" width="13.85546875" style="33" customWidth="1"/>
-    <col min="3" max="8" width="14.140625" style="33" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="33"/>
+    <col min="1" max="1" width="11.44140625" style="33"/>
+    <col min="2" max="2" width="13.88671875" style="33" customWidth="1"/>
+    <col min="3" max="8" width="14.109375" style="33" customWidth="1"/>
+    <col min="9" max="16384" width="11.44140625" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C1" s="33" t="s">
         <v>2</v>
       </c>
@@ -3412,7 +3457,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
@@ -3438,7 +3483,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -3467,7 +3512,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -3496,7 +3541,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -3525,7 +3570,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -3554,7 +3599,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>60</v>
       </c>
@@ -3583,7 +3628,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -3612,7 +3657,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -3641,7 +3686,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -3670,7 +3715,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -3699,7 +3744,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -3728,7 +3773,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -3757,7 +3802,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -3786,7 +3831,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -3815,7 +3860,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -3844,7 +3889,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -3873,7 +3918,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -3902,7 +3947,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -3931,7 +3976,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>78</v>
       </c>
@@ -3960,7 +4005,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -3989,7 +4034,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>78</v>
       </c>
@@ -4018,7 +4063,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>78</v>
       </c>
@@ -4047,7 +4092,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -4076,7 +4121,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>78</v>
       </c>
@@ -4105,7 +4150,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>78</v>
       </c>
@@ -4134,7 +4179,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -4163,7 +4208,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>78</v>
       </c>
@@ -4192,7 +4237,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>78</v>
       </c>
@@ -4221,7 +4266,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>78</v>
       </c>
@@ -4250,7 +4295,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>78</v>
       </c>
@@ -4279,7 +4324,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -4308,7 +4353,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>78</v>
       </c>
@@ -4337,7 +4382,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>78</v>
       </c>
@@ -4366,7 +4411,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>78</v>
       </c>
@@ -4395,7 +4440,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>78</v>
       </c>
@@ -4426,6 +4471,2649 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F87D2359-5081-43B1-AB89-5DA93CF5FD72}">
+  <dimension ref="A1:N63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N63" sqref="A63:N63"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="6" max="7" width="17.44140625" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="14.5546875" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="13" max="13" width="15.88671875" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="K1" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="L1" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="M1" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="N1" s="36" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B2" s="38">
+        <v>10</v>
+      </c>
+      <c r="C2" s="39">
+        <v>45</v>
+      </c>
+      <c r="D2" s="39">
+        <v>51</v>
+      </c>
+      <c r="E2" s="37">
+        <v>69.5</v>
+      </c>
+      <c r="F2" s="39">
+        <v>79</v>
+      </c>
+      <c r="G2" s="39"/>
+      <c r="H2">
+        <v>2020</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>897</v>
+      </c>
+      <c r="K2">
+        <v>43</v>
+      </c>
+      <c r="L2">
+        <v>50</v>
+      </c>
+      <c r="M2">
+        <v>66</v>
+      </c>
+      <c r="N2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B3" s="38">
+        <v>11</v>
+      </c>
+      <c r="C3" s="39">
+        <v>47</v>
+      </c>
+      <c r="D3" s="39">
+        <v>58</v>
+      </c>
+      <c r="E3" s="39">
+        <v>67</v>
+      </c>
+      <c r="F3" s="39">
+        <v>80</v>
+      </c>
+      <c r="G3" s="39"/>
+      <c r="H3">
+        <v>2020</v>
+      </c>
+      <c r="I3">
+        <v>11</v>
+      </c>
+      <c r="J3">
+        <v>6429</v>
+      </c>
+      <c r="K3">
+        <v>45</v>
+      </c>
+      <c r="L3">
+        <v>57</v>
+      </c>
+      <c r="M3">
+        <v>66</v>
+      </c>
+      <c r="N3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B4" s="38">
+        <v>12</v>
+      </c>
+      <c r="C4" s="39">
+        <v>47</v>
+      </c>
+      <c r="D4" s="39">
+        <v>64</v>
+      </c>
+      <c r="E4" s="39">
+        <v>69</v>
+      </c>
+      <c r="F4" s="39">
+        <v>80</v>
+      </c>
+      <c r="G4" s="39"/>
+      <c r="H4">
+        <v>2020</v>
+      </c>
+      <c r="I4">
+        <v>12</v>
+      </c>
+      <c r="J4">
+        <v>22408</v>
+      </c>
+      <c r="K4">
+        <v>45</v>
+      </c>
+      <c r="L4">
+        <v>63</v>
+      </c>
+      <c r="M4">
+        <v>67</v>
+      </c>
+      <c r="N4">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B5" s="38">
+        <v>13</v>
+      </c>
+      <c r="C5" s="39">
+        <v>49</v>
+      </c>
+      <c r="D5" s="39">
+        <v>69</v>
+      </c>
+      <c r="E5" s="39">
+        <v>70</v>
+      </c>
+      <c r="F5" s="39">
+        <v>80</v>
+      </c>
+      <c r="G5" s="39"/>
+      <c r="H5">
+        <v>2020</v>
+      </c>
+      <c r="I5">
+        <v>13</v>
+      </c>
+      <c r="J5">
+        <v>33970</v>
+      </c>
+      <c r="K5">
+        <v>48</v>
+      </c>
+      <c r="L5">
+        <v>65</v>
+      </c>
+      <c r="M5">
+        <v>68</v>
+      </c>
+      <c r="N5">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B6" s="38">
+        <v>14</v>
+      </c>
+      <c r="C6" s="39">
+        <v>52</v>
+      </c>
+      <c r="D6" s="39">
+        <v>72</v>
+      </c>
+      <c r="E6" s="39">
+        <v>71</v>
+      </c>
+      <c r="F6" s="39">
+        <v>83</v>
+      </c>
+      <c r="G6" s="39"/>
+      <c r="H6">
+        <v>2020</v>
+      </c>
+      <c r="I6">
+        <v>14</v>
+      </c>
+      <c r="J6">
+        <v>36052</v>
+      </c>
+      <c r="K6">
+        <v>51</v>
+      </c>
+      <c r="L6">
+        <v>68</v>
+      </c>
+      <c r="M6">
+        <v>68</v>
+      </c>
+      <c r="N6">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B7" s="38">
+        <v>15</v>
+      </c>
+      <c r="C7" s="39">
+        <v>52</v>
+      </c>
+      <c r="D7" s="39">
+        <v>74</v>
+      </c>
+      <c r="E7" s="39">
+        <v>71</v>
+      </c>
+      <c r="F7" s="39">
+        <v>83</v>
+      </c>
+      <c r="G7" s="39"/>
+      <c r="H7">
+        <v>2020</v>
+      </c>
+      <c r="I7">
+        <v>15</v>
+      </c>
+      <c r="J7">
+        <v>27156</v>
+      </c>
+      <c r="K7">
+        <v>52</v>
+      </c>
+      <c r="L7">
+        <v>69</v>
+      </c>
+      <c r="M7">
+        <v>69</v>
+      </c>
+      <c r="N7">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B8" s="38">
+        <v>16</v>
+      </c>
+      <c r="C8" s="39">
+        <v>52</v>
+      </c>
+      <c r="D8" s="39">
+        <v>75</v>
+      </c>
+      <c r="E8" s="39">
+        <v>71</v>
+      </c>
+      <c r="F8" s="39">
+        <v>83</v>
+      </c>
+      <c r="G8" s="39"/>
+      <c r="H8">
+        <v>2020</v>
+      </c>
+      <c r="I8">
+        <v>16</v>
+      </c>
+      <c r="J8">
+        <v>17342</v>
+      </c>
+      <c r="K8">
+        <v>51</v>
+      </c>
+      <c r="L8">
+        <v>69</v>
+      </c>
+      <c r="M8">
+        <v>68</v>
+      </c>
+      <c r="N8">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B9" s="38">
+        <v>17</v>
+      </c>
+      <c r="C9" s="39">
+        <v>50</v>
+      </c>
+      <c r="D9" s="37">
+        <v>74.5</v>
+      </c>
+      <c r="E9" s="39">
+        <v>71</v>
+      </c>
+      <c r="F9" s="39">
+        <v>84</v>
+      </c>
+      <c r="G9" s="39"/>
+      <c r="H9">
+        <v>2020</v>
+      </c>
+      <c r="I9">
+        <v>17</v>
+      </c>
+      <c r="J9">
+        <v>12359</v>
+      </c>
+      <c r="K9">
+        <v>50</v>
+      </c>
+      <c r="L9">
+        <v>67</v>
+      </c>
+      <c r="M9">
+        <v>68</v>
+      </c>
+      <c r="N9">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B10" s="38">
+        <v>18</v>
+      </c>
+      <c r="C10" s="39">
+        <v>48</v>
+      </c>
+      <c r="D10" s="39">
+        <v>72</v>
+      </c>
+      <c r="E10" s="39">
+        <v>70</v>
+      </c>
+      <c r="F10" s="39">
+        <v>82</v>
+      </c>
+      <c r="G10" s="39"/>
+      <c r="H10">
+        <v>2020</v>
+      </c>
+      <c r="I10">
+        <v>18</v>
+      </c>
+      <c r="J10">
+        <v>7438</v>
+      </c>
+      <c r="K10">
+        <v>48</v>
+      </c>
+      <c r="L10">
+        <v>66</v>
+      </c>
+      <c r="M10">
+        <v>68</v>
+      </c>
+      <c r="N10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B11" s="38">
+        <v>19</v>
+      </c>
+      <c r="C11" s="39">
+        <v>46</v>
+      </c>
+      <c r="D11" s="39">
+        <v>71</v>
+      </c>
+      <c r="E11" s="39">
+        <v>71</v>
+      </c>
+      <c r="F11" s="39">
+        <v>82</v>
+      </c>
+      <c r="G11" s="39"/>
+      <c r="H11">
+        <v>2020</v>
+      </c>
+      <c r="I11">
+        <v>19</v>
+      </c>
+      <c r="J11">
+        <v>6239</v>
+      </c>
+      <c r="K11">
+        <v>47</v>
+      </c>
+      <c r="L11">
+        <v>66</v>
+      </c>
+      <c r="M11">
+        <v>69</v>
+      </c>
+      <c r="N11">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B12" s="38">
+        <v>20</v>
+      </c>
+      <c r="C12" s="39">
+        <v>44</v>
+      </c>
+      <c r="D12" s="39">
+        <v>71</v>
+      </c>
+      <c r="E12" s="39">
+        <v>74</v>
+      </c>
+      <c r="F12" s="39">
+        <v>84</v>
+      </c>
+      <c r="G12" s="39"/>
+      <c r="H12">
+        <v>2020</v>
+      </c>
+      <c r="I12">
+        <v>20</v>
+      </c>
+      <c r="J12">
+        <v>4761</v>
+      </c>
+      <c r="K12">
+        <v>45</v>
+      </c>
+      <c r="L12">
+        <v>64</v>
+      </c>
+      <c r="M12">
+        <v>70</v>
+      </c>
+      <c r="N12">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B13" s="38">
+        <v>21</v>
+      </c>
+      <c r="C13" s="39">
+        <v>41</v>
+      </c>
+      <c r="D13" s="39">
+        <v>69</v>
+      </c>
+      <c r="E13" s="39">
+        <v>72</v>
+      </c>
+      <c r="F13" s="39">
+        <v>84</v>
+      </c>
+      <c r="G13" s="39"/>
+      <c r="H13">
+        <v>2020</v>
+      </c>
+      <c r="I13">
+        <v>21</v>
+      </c>
+      <c r="J13">
+        <v>3601</v>
+      </c>
+      <c r="K13">
+        <v>44</v>
+      </c>
+      <c r="L13">
+        <v>65</v>
+      </c>
+      <c r="M13">
+        <v>72</v>
+      </c>
+      <c r="N13">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B14" s="38">
+        <v>22</v>
+      </c>
+      <c r="C14" s="39">
+        <v>40</v>
+      </c>
+      <c r="D14" s="37">
+        <v>67.5</v>
+      </c>
+      <c r="E14" s="39">
+        <v>70</v>
+      </c>
+      <c r="F14" s="39">
+        <v>80</v>
+      </c>
+      <c r="G14" s="39"/>
+      <c r="H14">
+        <v>2020</v>
+      </c>
+      <c r="I14">
+        <v>22</v>
+      </c>
+      <c r="J14">
+        <v>3207</v>
+      </c>
+      <c r="K14">
+        <v>42</v>
+      </c>
+      <c r="L14">
+        <v>63</v>
+      </c>
+      <c r="M14">
+        <v>65</v>
+      </c>
+      <c r="N14">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B15" s="38">
+        <v>23</v>
+      </c>
+      <c r="C15" s="39">
+        <v>36</v>
+      </c>
+      <c r="D15" s="39">
+        <v>63</v>
+      </c>
+      <c r="E15" s="39">
+        <v>60</v>
+      </c>
+      <c r="F15" s="39">
+        <v>80</v>
+      </c>
+      <c r="G15" s="39"/>
+      <c r="H15">
+        <v>2020</v>
+      </c>
+      <c r="I15">
+        <v>23</v>
+      </c>
+      <c r="J15">
+        <v>2351</v>
+      </c>
+      <c r="K15">
+        <v>39</v>
+      </c>
+      <c r="L15">
+        <v>60</v>
+      </c>
+      <c r="M15">
+        <v>58</v>
+      </c>
+      <c r="N15">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B16" s="38">
+        <v>24</v>
+      </c>
+      <c r="C16" s="39">
+        <v>34</v>
+      </c>
+      <c r="D16" s="39">
+        <v>59</v>
+      </c>
+      <c r="E16" s="37">
+        <v>61.5</v>
+      </c>
+      <c r="F16" s="39">
+        <v>83</v>
+      </c>
+      <c r="G16" s="39"/>
+      <c r="H16">
+        <v>2020</v>
+      </c>
+      <c r="I16">
+        <v>24</v>
+      </c>
+      <c r="J16">
+        <v>2342</v>
+      </c>
+      <c r="K16">
+        <v>37</v>
+      </c>
+      <c r="L16">
+        <v>56</v>
+      </c>
+      <c r="M16">
+        <v>60</v>
+      </c>
+      <c r="N16">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B17" s="38">
+        <v>25</v>
+      </c>
+      <c r="C17" s="39">
+        <v>36</v>
+      </c>
+      <c r="D17" s="39">
+        <v>55</v>
+      </c>
+      <c r="E17" s="37">
+        <v>62.5</v>
+      </c>
+      <c r="F17" s="39">
+        <v>76</v>
+      </c>
+      <c r="G17" s="39"/>
+      <c r="H17">
+        <v>2020</v>
+      </c>
+      <c r="I17">
+        <v>25</v>
+      </c>
+      <c r="J17">
+        <v>4126</v>
+      </c>
+      <c r="K17">
+        <v>36</v>
+      </c>
+      <c r="L17">
+        <v>56</v>
+      </c>
+      <c r="M17">
+        <v>65</v>
+      </c>
+      <c r="N17">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B18" s="38">
+        <v>26</v>
+      </c>
+      <c r="C18" s="39">
+        <v>36</v>
+      </c>
+      <c r="D18" s="39">
+        <v>57</v>
+      </c>
+      <c r="E18" s="39">
+        <v>66</v>
+      </c>
+      <c r="F18" s="39">
+        <v>78</v>
+      </c>
+      <c r="G18" s="39"/>
+      <c r="H18">
+        <v>2020</v>
+      </c>
+      <c r="I18">
+        <v>26</v>
+      </c>
+      <c r="J18">
+        <v>3211</v>
+      </c>
+      <c r="K18">
+        <v>37</v>
+      </c>
+      <c r="L18">
+        <v>56</v>
+      </c>
+      <c r="M18">
+        <v>63</v>
+      </c>
+      <c r="N18">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B19" s="38">
+        <v>27</v>
+      </c>
+      <c r="C19" s="39">
+        <v>35</v>
+      </c>
+      <c r="D19" s="39">
+        <v>53</v>
+      </c>
+      <c r="E19" s="39">
+        <v>66</v>
+      </c>
+      <c r="F19" s="37">
+        <v>77.5</v>
+      </c>
+      <c r="G19" s="37"/>
+      <c r="H19">
+        <v>2020</v>
+      </c>
+      <c r="I19">
+        <v>27</v>
+      </c>
+      <c r="J19">
+        <v>2690</v>
+      </c>
+      <c r="K19">
+        <v>36</v>
+      </c>
+      <c r="L19">
+        <v>54</v>
+      </c>
+      <c r="M19">
+        <v>63</v>
+      </c>
+      <c r="N19">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B20" s="38">
+        <v>28</v>
+      </c>
+      <c r="C20" s="39">
+        <v>34</v>
+      </c>
+      <c r="D20" s="39">
+        <v>54</v>
+      </c>
+      <c r="E20" s="39">
+        <v>63</v>
+      </c>
+      <c r="F20" s="39">
+        <v>79</v>
+      </c>
+      <c r="G20" s="39"/>
+      <c r="H20">
+        <v>2020</v>
+      </c>
+      <c r="I20">
+        <v>28</v>
+      </c>
+      <c r="J20">
+        <v>2426</v>
+      </c>
+      <c r="K20">
+        <v>36</v>
+      </c>
+      <c r="L20">
+        <v>54</v>
+      </c>
+      <c r="M20">
+        <v>60</v>
+      </c>
+      <c r="N20">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B21" s="38">
+        <v>29</v>
+      </c>
+      <c r="C21" s="39">
+        <v>34</v>
+      </c>
+      <c r="D21" s="39">
+        <v>54</v>
+      </c>
+      <c r="E21" s="39">
+        <v>65</v>
+      </c>
+      <c r="F21" s="39">
+        <v>81</v>
+      </c>
+      <c r="G21" s="39"/>
+      <c r="H21">
+        <v>2020</v>
+      </c>
+      <c r="I21">
+        <v>29</v>
+      </c>
+      <c r="J21">
+        <v>3016</v>
+      </c>
+      <c r="K21">
+        <v>36</v>
+      </c>
+      <c r="L21">
+        <v>53</v>
+      </c>
+      <c r="M21">
+        <v>64</v>
+      </c>
+      <c r="N21">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B22" s="38">
+        <v>30</v>
+      </c>
+      <c r="C22" s="39">
+        <v>35</v>
+      </c>
+      <c r="D22" s="39">
+        <v>56</v>
+      </c>
+      <c r="E22" s="39">
+        <v>64</v>
+      </c>
+      <c r="F22" s="39">
+        <v>79</v>
+      </c>
+      <c r="G22" s="39"/>
+      <c r="H22">
+        <v>2020</v>
+      </c>
+      <c r="I22">
+        <v>30</v>
+      </c>
+      <c r="J22">
+        <v>3929</v>
+      </c>
+      <c r="K22">
+        <v>36</v>
+      </c>
+      <c r="L22">
+        <v>54</v>
+      </c>
+      <c r="M22">
+        <v>60</v>
+      </c>
+      <c r="N22">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B23" s="38">
+        <v>31</v>
+      </c>
+      <c r="C23" s="39">
+        <v>34</v>
+      </c>
+      <c r="D23" s="39">
+        <v>58</v>
+      </c>
+      <c r="E23" s="39">
+        <v>59</v>
+      </c>
+      <c r="F23" s="37">
+        <v>82.5</v>
+      </c>
+      <c r="G23" s="37"/>
+      <c r="H23">
+        <v>2020</v>
+      </c>
+      <c r="I23">
+        <v>31</v>
+      </c>
+      <c r="J23">
+        <v>4823</v>
+      </c>
+      <c r="K23">
+        <v>36</v>
+      </c>
+      <c r="L23">
+        <v>57</v>
+      </c>
+      <c r="M23">
+        <v>60</v>
+      </c>
+      <c r="N23">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B24" s="38">
+        <v>32</v>
+      </c>
+      <c r="C24" s="39">
+        <v>32</v>
+      </c>
+      <c r="D24" s="39">
+        <v>56</v>
+      </c>
+      <c r="E24" s="39">
+        <v>72</v>
+      </c>
+      <c r="F24" s="39">
+        <v>85</v>
+      </c>
+      <c r="G24" s="39"/>
+      <c r="H24">
+        <v>2020</v>
+      </c>
+      <c r="I24">
+        <v>32</v>
+      </c>
+      <c r="J24">
+        <v>6054</v>
+      </c>
+      <c r="K24">
+        <v>34</v>
+      </c>
+      <c r="L24">
+        <v>54</v>
+      </c>
+      <c r="M24">
+        <v>68</v>
+      </c>
+      <c r="N24">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B25" s="38">
+        <v>33</v>
+      </c>
+      <c r="C25" s="39">
+        <v>30</v>
+      </c>
+      <c r="D25" s="39">
+        <v>56</v>
+      </c>
+      <c r="E25" s="37">
+        <v>62.5</v>
+      </c>
+      <c r="F25" s="39">
+        <v>83</v>
+      </c>
+      <c r="G25" s="39"/>
+      <c r="H25">
+        <v>2020</v>
+      </c>
+      <c r="I25">
+        <v>33</v>
+      </c>
+      <c r="J25">
+        <v>7949</v>
+      </c>
+      <c r="K25">
+        <v>32</v>
+      </c>
+      <c r="L25">
+        <v>53</v>
+      </c>
+      <c r="M25">
+        <v>61</v>
+      </c>
+      <c r="N25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B26" s="38">
+        <v>34</v>
+      </c>
+      <c r="C26" s="39">
+        <v>29</v>
+      </c>
+      <c r="D26" s="39">
+        <v>51</v>
+      </c>
+      <c r="E26" s="39">
+        <v>63</v>
+      </c>
+      <c r="F26" s="39">
+        <v>75</v>
+      </c>
+      <c r="G26" s="39"/>
+      <c r="H26">
+        <v>2020</v>
+      </c>
+      <c r="I26">
+        <v>34</v>
+      </c>
+      <c r="J26">
+        <v>9591</v>
+      </c>
+      <c r="K26">
+        <v>32</v>
+      </c>
+      <c r="L26">
+        <v>50</v>
+      </c>
+      <c r="M26">
+        <v>62</v>
+      </c>
+      <c r="N26">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B27" s="38">
+        <v>35</v>
+      </c>
+      <c r="C27" s="39">
+        <v>29</v>
+      </c>
+      <c r="D27" s="37">
+        <v>51.5</v>
+      </c>
+      <c r="E27" s="37">
+        <v>57.5</v>
+      </c>
+      <c r="F27" s="37">
+        <v>76.5</v>
+      </c>
+      <c r="G27" s="37"/>
+      <c r="H27">
+        <v>2020</v>
+      </c>
+      <c r="I27">
+        <v>35</v>
+      </c>
+      <c r="J27">
+        <v>8820</v>
+      </c>
+      <c r="K27">
+        <v>32</v>
+      </c>
+      <c r="L27">
+        <v>51</v>
+      </c>
+      <c r="M27">
+        <v>58</v>
+      </c>
+      <c r="N27">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B28" s="38">
+        <v>36</v>
+      </c>
+      <c r="C28" s="39">
+        <v>30</v>
+      </c>
+      <c r="D28" s="39">
+        <v>55</v>
+      </c>
+      <c r="E28" s="39">
+        <v>64</v>
+      </c>
+      <c r="F28" s="37">
+        <v>78.5</v>
+      </c>
+      <c r="G28" s="37"/>
+      <c r="H28">
+        <v>2020</v>
+      </c>
+      <c r="I28">
+        <v>36</v>
+      </c>
+      <c r="J28">
+        <v>8615</v>
+      </c>
+      <c r="K28">
+        <v>33</v>
+      </c>
+      <c r="L28">
+        <v>54</v>
+      </c>
+      <c r="M28">
+        <v>64</v>
+      </c>
+      <c r="N28">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B29" s="38">
+        <v>37</v>
+      </c>
+      <c r="C29" s="39">
+        <v>32</v>
+      </c>
+      <c r="D29" s="39">
+        <v>60</v>
+      </c>
+      <c r="E29" s="39">
+        <v>71</v>
+      </c>
+      <c r="F29" s="39">
+        <v>81</v>
+      </c>
+      <c r="G29" s="39"/>
+      <c r="H29">
+        <v>2020</v>
+      </c>
+      <c r="I29">
+        <v>37</v>
+      </c>
+      <c r="J29">
+        <v>9768</v>
+      </c>
+      <c r="K29">
+        <v>35</v>
+      </c>
+      <c r="L29">
+        <v>57</v>
+      </c>
+      <c r="M29">
+        <v>65</v>
+      </c>
+      <c r="N29">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B30" s="38">
+        <v>38</v>
+      </c>
+      <c r="C30" s="39">
+        <v>33</v>
+      </c>
+      <c r="D30" s="39">
+        <v>60</v>
+      </c>
+      <c r="E30" s="37">
+        <v>61.5</v>
+      </c>
+      <c r="F30" s="39">
+        <v>81</v>
+      </c>
+      <c r="G30" s="39"/>
+      <c r="H30">
+        <v>2020</v>
+      </c>
+      <c r="I30">
+        <v>38</v>
+      </c>
+      <c r="J30">
+        <v>12294</v>
+      </c>
+      <c r="K30">
+        <v>36</v>
+      </c>
+      <c r="L30">
+        <v>59</v>
+      </c>
+      <c r="M30">
+        <v>60</v>
+      </c>
+      <c r="N30">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B31" s="38">
+        <v>39</v>
+      </c>
+      <c r="C31" s="39">
+        <v>34</v>
+      </c>
+      <c r="D31" s="39">
+        <v>61</v>
+      </c>
+      <c r="E31" s="37">
+        <v>68.5</v>
+      </c>
+      <c r="F31" s="39">
+        <v>83</v>
+      </c>
+      <c r="G31" s="39"/>
+      <c r="H31">
+        <v>2020</v>
+      </c>
+      <c r="I31">
+        <v>39</v>
+      </c>
+      <c r="J31">
+        <v>13064</v>
+      </c>
+      <c r="K31">
+        <v>37</v>
+      </c>
+      <c r="L31">
+        <v>58</v>
+      </c>
+      <c r="M31">
+        <v>65</v>
+      </c>
+      <c r="N31">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B32" s="38">
+        <v>40</v>
+      </c>
+      <c r="C32" s="39">
+        <v>35</v>
+      </c>
+      <c r="D32" s="39">
+        <v>61</v>
+      </c>
+      <c r="E32" s="39">
+        <v>68</v>
+      </c>
+      <c r="F32" s="39">
+        <v>82</v>
+      </c>
+      <c r="G32" s="39"/>
+      <c r="H32">
+        <v>2020</v>
+      </c>
+      <c r="I32">
+        <v>40</v>
+      </c>
+      <c r="J32">
+        <v>15928</v>
+      </c>
+      <c r="K32">
+        <v>38</v>
+      </c>
+      <c r="L32">
+        <v>58</v>
+      </c>
+      <c r="M32">
+        <v>66</v>
+      </c>
+      <c r="N32">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B33" s="38">
+        <v>41</v>
+      </c>
+      <c r="C33" s="39">
+        <v>37</v>
+      </c>
+      <c r="D33" s="39">
+        <v>62</v>
+      </c>
+      <c r="E33" s="39">
+        <v>69</v>
+      </c>
+      <c r="F33" s="39">
+        <v>82</v>
+      </c>
+      <c r="G33" s="39"/>
+      <c r="H33">
+        <v>2020</v>
+      </c>
+      <c r="I33">
+        <v>41</v>
+      </c>
+      <c r="J33">
+        <v>26126</v>
+      </c>
+      <c r="K33">
+        <v>39</v>
+      </c>
+      <c r="L33">
+        <v>59</v>
+      </c>
+      <c r="M33">
+        <v>67</v>
+      </c>
+      <c r="N33">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B34" s="38">
+        <v>42</v>
+      </c>
+      <c r="C34" s="39">
+        <v>37</v>
+      </c>
+      <c r="D34" s="39">
+        <v>65</v>
+      </c>
+      <c r="E34" s="39">
+        <v>69</v>
+      </c>
+      <c r="F34" s="39">
+        <v>83</v>
+      </c>
+      <c r="G34" s="39"/>
+      <c r="H34">
+        <v>2020</v>
+      </c>
+      <c r="I34">
+        <v>42</v>
+      </c>
+      <c r="J34">
+        <v>42086</v>
+      </c>
+      <c r="K34">
+        <v>39</v>
+      </c>
+      <c r="L34">
+        <v>61</v>
+      </c>
+      <c r="M34">
+        <v>66</v>
+      </c>
+      <c r="N34">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B35" s="38">
+        <v>43</v>
+      </c>
+      <c r="C35" s="39">
+        <v>39</v>
+      </c>
+      <c r="D35" s="39">
+        <v>67</v>
+      </c>
+      <c r="E35" s="39">
+        <v>72</v>
+      </c>
+      <c r="F35" s="39">
+        <v>83</v>
+      </c>
+      <c r="G35" s="39"/>
+      <c r="H35">
+        <v>2020</v>
+      </c>
+      <c r="I35">
+        <v>43</v>
+      </c>
+      <c r="J35">
+        <v>74811</v>
+      </c>
+      <c r="K35">
+        <v>40</v>
+      </c>
+      <c r="L35">
+        <v>63</v>
+      </c>
+      <c r="M35">
+        <v>68</v>
+      </c>
+      <c r="N35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B36" s="38">
+        <v>44</v>
+      </c>
+      <c r="C36" s="39">
+        <v>40</v>
+      </c>
+      <c r="D36" s="39">
+        <v>68</v>
+      </c>
+      <c r="E36" s="39">
+        <v>71</v>
+      </c>
+      <c r="F36" s="39">
+        <v>83</v>
+      </c>
+      <c r="G36" s="39"/>
+      <c r="H36">
+        <v>2020</v>
+      </c>
+      <c r="I36">
+        <v>44</v>
+      </c>
+      <c r="J36">
+        <v>111078</v>
+      </c>
+      <c r="K36">
+        <v>41</v>
+      </c>
+      <c r="L36">
+        <v>64</v>
+      </c>
+      <c r="M36">
+        <v>68</v>
+      </c>
+      <c r="N36">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B37" s="38">
+        <v>45</v>
+      </c>
+      <c r="C37" s="39">
+        <v>40</v>
+      </c>
+      <c r="D37" s="39">
+        <v>70</v>
+      </c>
+      <c r="E37" s="37">
+        <v>72.5</v>
+      </c>
+      <c r="F37" s="39">
+        <v>83</v>
+      </c>
+      <c r="G37" s="39"/>
+      <c r="H37">
+        <v>2020</v>
+      </c>
+      <c r="I37">
+        <v>45</v>
+      </c>
+      <c r="J37">
+        <v>125794</v>
+      </c>
+      <c r="K37">
+        <v>41</v>
+      </c>
+      <c r="L37">
+        <v>64</v>
+      </c>
+      <c r="M37">
+        <v>69</v>
+      </c>
+      <c r="N37">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A38" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B38" s="38">
+        <v>46</v>
+      </c>
+      <c r="C38" s="39">
+        <v>41</v>
+      </c>
+      <c r="D38" s="39">
+        <v>72</v>
+      </c>
+      <c r="E38" s="39">
+        <v>73</v>
+      </c>
+      <c r="F38" s="39">
+        <v>84</v>
+      </c>
+      <c r="G38" s="39"/>
+      <c r="H38">
+        <v>2020</v>
+      </c>
+      <c r="I38">
+        <v>46</v>
+      </c>
+      <c r="J38">
+        <v>127839</v>
+      </c>
+      <c r="K38">
+        <v>42</v>
+      </c>
+      <c r="L38">
+        <v>66</v>
+      </c>
+      <c r="M38">
+        <v>70</v>
+      </c>
+      <c r="N38">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A39" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B39" s="38">
+        <v>47</v>
+      </c>
+      <c r="C39" s="39">
+        <v>42</v>
+      </c>
+      <c r="D39" s="39">
+        <v>73</v>
+      </c>
+      <c r="E39" s="39">
+        <v>72</v>
+      </c>
+      <c r="F39" s="39">
+        <v>84</v>
+      </c>
+      <c r="G39" s="39"/>
+      <c r="H39">
+        <v>2020</v>
+      </c>
+      <c r="I39">
+        <v>47</v>
+      </c>
+      <c r="J39">
+        <v>128445</v>
+      </c>
+      <c r="K39">
+        <v>43</v>
+      </c>
+      <c r="L39">
+        <v>67</v>
+      </c>
+      <c r="M39">
+        <v>69</v>
+      </c>
+      <c r="N39">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A40" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B40" s="38">
+        <v>48</v>
+      </c>
+      <c r="C40" s="39">
+        <v>43</v>
+      </c>
+      <c r="D40" s="39">
+        <v>73</v>
+      </c>
+      <c r="E40" s="39">
+        <v>71</v>
+      </c>
+      <c r="F40" s="39">
+        <v>84</v>
+      </c>
+      <c r="G40" s="39"/>
+      <c r="H40">
+        <v>2020</v>
+      </c>
+      <c r="I40">
+        <v>48</v>
+      </c>
+      <c r="J40">
+        <v>123288</v>
+      </c>
+      <c r="K40">
+        <v>44</v>
+      </c>
+      <c r="L40">
+        <v>67</v>
+      </c>
+      <c r="M40">
+        <v>69</v>
+      </c>
+      <c r="N40">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A41" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B41" s="38">
+        <v>49</v>
+      </c>
+      <c r="C41" s="39">
+        <v>44</v>
+      </c>
+      <c r="D41" s="39">
+        <v>75</v>
+      </c>
+      <c r="E41" s="39">
+        <v>73</v>
+      </c>
+      <c r="F41" s="39">
+        <v>84</v>
+      </c>
+      <c r="G41" s="39"/>
+      <c r="H41">
+        <v>2020</v>
+      </c>
+      <c r="I41">
+        <v>49</v>
+      </c>
+      <c r="J41">
+        <v>128489</v>
+      </c>
+      <c r="K41">
+        <v>45</v>
+      </c>
+      <c r="L41">
+        <v>69</v>
+      </c>
+      <c r="M41">
+        <v>70</v>
+      </c>
+      <c r="N41">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A42" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B42" s="38">
+        <v>50</v>
+      </c>
+      <c r="C42" s="39">
+        <v>45</v>
+      </c>
+      <c r="D42" s="39">
+        <v>76</v>
+      </c>
+      <c r="E42" s="39">
+        <v>73</v>
+      </c>
+      <c r="F42" s="39">
+        <v>84</v>
+      </c>
+      <c r="G42" s="39"/>
+      <c r="H42">
+        <v>2020</v>
+      </c>
+      <c r="I42">
+        <v>50</v>
+      </c>
+      <c r="J42">
+        <v>156489</v>
+      </c>
+      <c r="K42">
+        <v>46</v>
+      </c>
+      <c r="L42">
+        <v>69</v>
+      </c>
+      <c r="M42">
+        <v>70</v>
+      </c>
+      <c r="N42">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A43" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B43" s="38">
+        <v>51</v>
+      </c>
+      <c r="C43" s="39">
+        <v>47</v>
+      </c>
+      <c r="D43" s="39">
+        <v>76</v>
+      </c>
+      <c r="E43" s="39">
+        <v>74</v>
+      </c>
+      <c r="F43" s="39">
+        <v>84</v>
+      </c>
+      <c r="G43" s="39"/>
+      <c r="H43">
+        <v>2020</v>
+      </c>
+      <c r="I43">
+        <v>51</v>
+      </c>
+      <c r="J43">
+        <v>174879</v>
+      </c>
+      <c r="K43">
+        <v>46</v>
+      </c>
+      <c r="L43">
+        <v>69</v>
+      </c>
+      <c r="M43">
+        <v>71</v>
+      </c>
+      <c r="N43">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A44" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B44" s="38">
+        <v>52</v>
+      </c>
+      <c r="C44" s="39">
+        <v>48</v>
+      </c>
+      <c r="D44" s="39">
+        <v>77</v>
+      </c>
+      <c r="E44" s="39">
+        <v>73</v>
+      </c>
+      <c r="F44" s="39">
+        <v>84</v>
+      </c>
+      <c r="G44" s="39"/>
+      <c r="H44">
+        <v>2020</v>
+      </c>
+      <c r="I44">
+        <v>52</v>
+      </c>
+      <c r="J44">
+        <v>139154</v>
+      </c>
+      <c r="K44">
+        <v>48</v>
+      </c>
+      <c r="L44">
+        <v>70</v>
+      </c>
+      <c r="M44">
+        <v>71</v>
+      </c>
+      <c r="N44">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A45" s="38">
+        <v>2020</v>
+      </c>
+      <c r="B45" s="38">
+        <v>53</v>
+      </c>
+      <c r="C45" s="39">
+        <v>49</v>
+      </c>
+      <c r="D45" s="39">
+        <v>76</v>
+      </c>
+      <c r="E45" s="39">
+        <v>73</v>
+      </c>
+      <c r="F45" s="39">
+        <v>84</v>
+      </c>
+      <c r="G45" s="39"/>
+      <c r="H45">
+        <v>2020</v>
+      </c>
+      <c r="I45">
+        <v>53</v>
+      </c>
+      <c r="J45">
+        <v>123151</v>
+      </c>
+      <c r="K45">
+        <v>49</v>
+      </c>
+      <c r="L45">
+        <v>70</v>
+      </c>
+      <c r="M45">
+        <v>70</v>
+      </c>
+      <c r="N45">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A46" s="38">
+        <v>2021</v>
+      </c>
+      <c r="B46" s="38">
+        <v>1</v>
+      </c>
+      <c r="C46" s="39">
+        <v>48</v>
+      </c>
+      <c r="D46" s="39">
+        <v>77</v>
+      </c>
+      <c r="E46" s="39">
+        <v>73</v>
+      </c>
+      <c r="F46" s="39">
+        <v>84</v>
+      </c>
+      <c r="G46" s="39"/>
+      <c r="H46">
+        <v>2021</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="J46">
+        <v>145533</v>
+      </c>
+      <c r="K46">
+        <v>48</v>
+      </c>
+      <c r="L46">
+        <v>70</v>
+      </c>
+      <c r="M46">
+        <v>71</v>
+      </c>
+      <c r="N46">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A47" s="38">
+        <v>2021</v>
+      </c>
+      <c r="B47" s="38">
+        <v>2</v>
+      </c>
+      <c r="C47" s="39">
+        <v>48</v>
+      </c>
+      <c r="D47" s="39">
+        <v>77</v>
+      </c>
+      <c r="E47" s="39">
+        <v>75</v>
+      </c>
+      <c r="F47" s="39">
+        <v>84</v>
+      </c>
+      <c r="G47" s="39"/>
+      <c r="H47">
+        <v>2021</v>
+      </c>
+      <c r="I47">
+        <v>2</v>
+      </c>
+      <c r="J47">
+        <v>119049</v>
+      </c>
+      <c r="K47">
+        <v>48</v>
+      </c>
+      <c r="L47">
+        <v>70</v>
+      </c>
+      <c r="M47">
+        <v>72</v>
+      </c>
+      <c r="N47">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A48" s="38">
+        <v>2021</v>
+      </c>
+      <c r="B48" s="38">
+        <v>3</v>
+      </c>
+      <c r="C48" s="39">
+        <v>49</v>
+      </c>
+      <c r="D48" s="39">
+        <v>77</v>
+      </c>
+      <c r="E48" s="39">
+        <v>74</v>
+      </c>
+      <c r="F48" s="39">
+        <v>84</v>
+      </c>
+      <c r="G48" s="39"/>
+      <c r="H48">
+        <v>2021</v>
+      </c>
+      <c r="I48">
+        <v>3</v>
+      </c>
+      <c r="J48">
+        <v>95602</v>
+      </c>
+      <c r="K48">
+        <v>48</v>
+      </c>
+      <c r="L48">
+        <v>71</v>
+      </c>
+      <c r="M48">
+        <v>71</v>
+      </c>
+      <c r="N48">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A49" s="38">
+        <v>2021</v>
+      </c>
+      <c r="B49" s="38">
+        <v>4</v>
+      </c>
+      <c r="C49" s="39">
+        <v>48</v>
+      </c>
+      <c r="D49" s="39">
+        <v>76</v>
+      </c>
+      <c r="E49" s="37">
+        <v>73.5</v>
+      </c>
+      <c r="F49" s="39">
+        <v>83</v>
+      </c>
+      <c r="G49" s="39"/>
+      <c r="H49">
+        <v>2021</v>
+      </c>
+      <c r="I49">
+        <v>4</v>
+      </c>
+      <c r="J49">
+        <v>78250</v>
+      </c>
+      <c r="K49">
+        <v>48</v>
+      </c>
+      <c r="L49">
+        <v>70</v>
+      </c>
+      <c r="M49">
+        <v>70</v>
+      </c>
+      <c r="N49">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A50" s="38">
+        <v>2021</v>
+      </c>
+      <c r="B50" s="38">
+        <v>5</v>
+      </c>
+      <c r="C50" s="39">
+        <v>47</v>
+      </c>
+      <c r="D50" s="39">
+        <v>76</v>
+      </c>
+      <c r="E50" s="39">
+        <v>73</v>
+      </c>
+      <c r="F50" s="39">
+        <v>84</v>
+      </c>
+      <c r="G50" s="39"/>
+      <c r="H50">
+        <v>2021</v>
+      </c>
+      <c r="I50">
+        <v>5</v>
+      </c>
+      <c r="J50">
+        <v>64669</v>
+      </c>
+      <c r="K50">
+        <v>46</v>
+      </c>
+      <c r="L50">
+        <v>69</v>
+      </c>
+      <c r="M50">
+        <v>70</v>
+      </c>
+      <c r="N50">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A51" s="38">
+        <v>2021</v>
+      </c>
+      <c r="B51" s="38">
+        <v>6</v>
+      </c>
+      <c r="C51" s="39">
+        <v>45</v>
+      </c>
+      <c r="D51" s="39">
+        <v>74</v>
+      </c>
+      <c r="E51" s="39">
+        <v>73</v>
+      </c>
+      <c r="F51" s="39">
+        <v>83</v>
+      </c>
+      <c r="G51" s="39"/>
+      <c r="H51">
+        <v>2021</v>
+      </c>
+      <c r="I51">
+        <v>6</v>
+      </c>
+      <c r="J51">
+        <v>50861</v>
+      </c>
+      <c r="K51">
+        <v>45</v>
+      </c>
+      <c r="L51">
+        <v>69</v>
+      </c>
+      <c r="M51">
+        <v>69</v>
+      </c>
+      <c r="N51">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A52" s="38">
+        <v>2021</v>
+      </c>
+      <c r="B52" s="38">
+        <v>7</v>
+      </c>
+      <c r="C52" s="39">
+        <v>44</v>
+      </c>
+      <c r="D52" s="39">
+        <v>73</v>
+      </c>
+      <c r="E52" s="39">
+        <v>74</v>
+      </c>
+      <c r="F52" s="39">
+        <v>82</v>
+      </c>
+      <c r="G52" s="39"/>
+      <c r="H52">
+        <v>2021</v>
+      </c>
+      <c r="I52">
+        <v>7</v>
+      </c>
+      <c r="J52">
+        <v>52491</v>
+      </c>
+      <c r="K52">
+        <v>44</v>
+      </c>
+      <c r="L52">
+        <v>67</v>
+      </c>
+      <c r="M52">
+        <v>69</v>
+      </c>
+      <c r="N52">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A53" s="38">
+        <v>2021</v>
+      </c>
+      <c r="B53" s="38">
+        <v>8</v>
+      </c>
+      <c r="C53" s="39">
+        <v>42</v>
+      </c>
+      <c r="D53" s="39">
+        <v>71</v>
+      </c>
+      <c r="E53" s="39">
+        <v>71</v>
+      </c>
+      <c r="F53" s="39">
+        <v>82</v>
+      </c>
+      <c r="G53" s="39"/>
+      <c r="H53">
+        <v>2021</v>
+      </c>
+      <c r="I53">
+        <v>8</v>
+      </c>
+      <c r="J53">
+        <v>56450</v>
+      </c>
+      <c r="K53">
+        <v>42</v>
+      </c>
+      <c r="L53">
+        <v>66</v>
+      </c>
+      <c r="M53">
+        <v>67</v>
+      </c>
+      <c r="N53">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A54" s="38">
+        <v>2021</v>
+      </c>
+      <c r="B54" s="38">
+        <v>9</v>
+      </c>
+      <c r="C54" s="39">
+        <v>40</v>
+      </c>
+      <c r="D54" s="39">
+        <v>69</v>
+      </c>
+      <c r="E54" s="39">
+        <v>68</v>
+      </c>
+      <c r="F54" s="39">
+        <v>81</v>
+      </c>
+      <c r="G54" s="39"/>
+      <c r="H54">
+        <v>2021</v>
+      </c>
+      <c r="I54">
+        <v>9</v>
+      </c>
+      <c r="J54">
+        <v>58500</v>
+      </c>
+      <c r="K54">
+        <v>40</v>
+      </c>
+      <c r="L54">
+        <v>65</v>
+      </c>
+      <c r="M54">
+        <v>66</v>
+      </c>
+      <c r="N54">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A55" s="38">
+        <v>2021</v>
+      </c>
+      <c r="B55" s="38">
+        <v>10</v>
+      </c>
+      <c r="C55" s="39">
+        <v>39</v>
+      </c>
+      <c r="D55" s="39">
+        <v>67</v>
+      </c>
+      <c r="E55" s="39">
+        <v>67</v>
+      </c>
+      <c r="F55" s="39">
+        <v>81</v>
+      </c>
+      <c r="G55" s="39"/>
+      <c r="H55">
+        <v>2021</v>
+      </c>
+      <c r="I55">
+        <v>10</v>
+      </c>
+      <c r="J55">
+        <v>71456</v>
+      </c>
+      <c r="K55">
+        <v>39</v>
+      </c>
+      <c r="L55">
+        <v>63</v>
+      </c>
+      <c r="M55">
+        <v>66</v>
+      </c>
+      <c r="N55">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A56" s="38">
+        <v>2021</v>
+      </c>
+      <c r="B56" s="38">
+        <v>11</v>
+      </c>
+      <c r="C56" s="39">
+        <v>38</v>
+      </c>
+      <c r="D56" s="39">
+        <v>66</v>
+      </c>
+      <c r="E56" s="39">
+        <v>66</v>
+      </c>
+      <c r="F56" s="39">
+        <v>80</v>
+      </c>
+      <c r="G56" s="39"/>
+      <c r="H56">
+        <v>2021</v>
+      </c>
+      <c r="I56">
+        <v>11</v>
+      </c>
+      <c r="J56">
+        <v>92775</v>
+      </c>
+      <c r="K56">
+        <v>39</v>
+      </c>
+      <c r="L56">
+        <v>62</v>
+      </c>
+      <c r="M56">
+        <v>64</v>
+      </c>
+      <c r="N56">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A57" s="38">
+        <v>2021</v>
+      </c>
+      <c r="B57" s="38">
+        <v>12</v>
+      </c>
+      <c r="C57" s="39">
+        <v>38</v>
+      </c>
+      <c r="D57" s="39">
+        <v>65</v>
+      </c>
+      <c r="E57" s="39">
+        <v>68</v>
+      </c>
+      <c r="F57" s="39">
+        <v>79</v>
+      </c>
+      <c r="G57" s="39"/>
+      <c r="H57">
+        <v>2021</v>
+      </c>
+      <c r="I57">
+        <v>12</v>
+      </c>
+      <c r="J57">
+        <v>116596</v>
+      </c>
+      <c r="K57">
+        <v>38</v>
+      </c>
+      <c r="L57">
+        <v>61</v>
+      </c>
+      <c r="M57">
+        <v>65</v>
+      </c>
+      <c r="N57">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A58" s="38">
+        <v>2021</v>
+      </c>
+      <c r="B58" s="38">
+        <v>13</v>
+      </c>
+      <c r="C58" s="39">
+        <v>39</v>
+      </c>
+      <c r="D58" s="39">
+        <v>65</v>
+      </c>
+      <c r="E58" s="39">
+        <v>67</v>
+      </c>
+      <c r="F58" s="39">
+        <v>79</v>
+      </c>
+      <c r="G58" s="39"/>
+      <c r="H58">
+        <v>2021</v>
+      </c>
+      <c r="I58">
+        <v>13</v>
+      </c>
+      <c r="J58">
+        <v>110406</v>
+      </c>
+      <c r="K58">
+        <v>39</v>
+      </c>
+      <c r="L58">
+        <v>61</v>
+      </c>
+      <c r="M58">
+        <v>65</v>
+      </c>
+      <c r="N58">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A59" s="38">
+        <v>2021</v>
+      </c>
+      <c r="B59" s="38">
+        <v>14</v>
+      </c>
+      <c r="C59" s="39">
+        <v>39</v>
+      </c>
+      <c r="D59" s="39">
+        <v>63</v>
+      </c>
+      <c r="E59" s="39">
+        <v>67</v>
+      </c>
+      <c r="F59" s="39">
+        <v>79</v>
+      </c>
+      <c r="G59" s="39"/>
+      <c r="H59">
+        <v>2021</v>
+      </c>
+      <c r="I59">
+        <v>14</v>
+      </c>
+      <c r="J59">
+        <v>118519</v>
+      </c>
+      <c r="K59">
+        <v>39</v>
+      </c>
+      <c r="L59">
+        <v>60</v>
+      </c>
+      <c r="M59">
+        <v>65</v>
+      </c>
+      <c r="N59">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A60" s="38">
+        <v>2021</v>
+      </c>
+      <c r="B60" s="38">
+        <v>15</v>
+      </c>
+      <c r="C60" s="39">
+        <v>37</v>
+      </c>
+      <c r="D60" s="39">
+        <v>64</v>
+      </c>
+      <c r="E60" s="39">
+        <v>67</v>
+      </c>
+      <c r="F60" s="39">
+        <v>80</v>
+      </c>
+      <c r="G60" s="39"/>
+      <c r="H60">
+        <v>2021</v>
+      </c>
+      <c r="I60">
+        <v>15</v>
+      </c>
+      <c r="J60">
+        <v>142548</v>
+      </c>
+      <c r="K60">
+        <v>38</v>
+      </c>
+      <c r="L60">
+        <v>60</v>
+      </c>
+      <c r="M60">
+        <v>65</v>
+      </c>
+      <c r="N60">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A61" s="38">
+        <v>2021</v>
+      </c>
+      <c r="B61" s="38">
+        <v>16</v>
+      </c>
+      <c r="C61" s="39">
+        <v>37</v>
+      </c>
+      <c r="D61" s="39">
+        <v>63</v>
+      </c>
+      <c r="E61" s="39">
+        <v>66</v>
+      </c>
+      <c r="F61" s="39">
+        <v>80</v>
+      </c>
+      <c r="G61" s="39"/>
+      <c r="H61">
+        <v>2021</v>
+      </c>
+      <c r="I61">
+        <v>16</v>
+      </c>
+      <c r="J61">
+        <v>145336</v>
+      </c>
+      <c r="K61">
+        <v>37</v>
+      </c>
+      <c r="L61">
+        <v>60</v>
+      </c>
+      <c r="M61">
+        <v>63</v>
+      </c>
+      <c r="N61">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A62" s="38">
+        <v>2021</v>
+      </c>
+      <c r="B62" s="38">
+        <v>17</v>
+      </c>
+      <c r="C62" s="39">
+        <v>37</v>
+      </c>
+      <c r="D62" s="39">
+        <v>64</v>
+      </c>
+      <c r="E62" s="39">
+        <v>67</v>
+      </c>
+      <c r="F62" s="39">
+        <v>80</v>
+      </c>
+      <c r="G62" s="39"/>
+      <c r="H62">
+        <v>2021</v>
+      </c>
+      <c r="I62">
+        <v>17</v>
+      </c>
+      <c r="J62">
+        <v>124151</v>
+      </c>
+      <c r="K62">
+        <v>37</v>
+      </c>
+      <c r="L62">
+        <v>60</v>
+      </c>
+      <c r="M62">
+        <v>64</v>
+      </c>
+      <c r="N62">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A63" s="38"/>
+      <c r="B63" s="38"/>
+      <c r="C63" s="39"/>
+      <c r="D63" s="37"/>
+      <c r="E63" s="39"/>
+      <c r="F63" s="39"/>
+      <c r="G63" s="39"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>